<commit_message>
Updated input and output files along with script
</commit_message>
<xml_diff>
--- a/Output/Qutation.xlsx
+++ b/Output/Qutation.xlsx
@@ -958,7 +958,7 @@
     <row r="5" ht="22" customHeight="1">
       <c r="A5" s="5" t="inlineStr">
         <is>
-          <t>7 MONTH DECK STORES</t>
+          <t>Equipment and Materials</t>
         </is>
       </c>
     </row>
@@ -1087,7 +1087,7 @@
       </c>
       <c r="B10" s="49" t="inlineStr">
         <is>
-          <t>NON SKID SHEET MESH, WIDTH 800MM</t>
+          <t>CONCRETE MIXER, 220V, 150L CAPACITY</t>
         </is>
       </c>
       <c r="C10" s="50" t="n"/>
@@ -1095,17 +1095,17 @@
       <c r="E10" s="49" t="n"/>
       <c r="F10" s="49" t="inlineStr">
         <is>
-          <t>150691 IMPA MAKER: IMPA CATALOG</t>
+          <t>617127 CONCRETE150</t>
         </is>
       </c>
       <c r="G10" s="49" t="n"/>
       <c r="H10" s="49" t="n"/>
       <c r="I10" s="48" t="n">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="J10" s="48" t="inlineStr">
         <is>
-          <t>MTR</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K10" s="52" t="n"/>
@@ -1122,7 +1122,7 @@
       </c>
       <c r="B11" s="49" t="inlineStr">
         <is>
-          <t>CURTAIN SHOWER WITH FURTHER, DETAIL</t>
+          <t>EXCAVATOR, CATERPILLAR, 10 TON</t>
         </is>
       </c>
       <c r="C11" s="50" t="n"/>
@@ -1130,17 +1130,17 @@
       <c r="E11" s="49" t="n"/>
       <c r="F11" s="49" t="inlineStr">
         <is>
-          <t>150714 IMPA MAKER: IMPA CATALOG</t>
+          <t>617128 EXCAVATOR10T</t>
         </is>
       </c>
       <c r="G11" s="49" t="n"/>
       <c r="H11" s="49" t="n"/>
       <c r="I11" s="48" t="n">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="J11" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K11" s="52" t="n"/>
@@ -1154,7 +1154,7 @@
       </c>
       <c r="B12" s="49" t="inlineStr">
         <is>
-          <t>NAPKIN PAPER TABLE 2-PLY, 330MM2 2000S</t>
+          <t>BACKHOE LOADER, KOMATSU, 4X4</t>
         </is>
       </c>
       <c r="C12" s="50" t="n"/>
@@ -1162,17 +1162,17 @@
       <c r="E12" s="49" t="n"/>
       <c r="F12" s="49" t="inlineStr">
         <is>
-          <t>171476 IMPA MAKER: IMPA CATALOG</t>
+          <t>617129 BACKHOE4X4</t>
         </is>
       </c>
       <c r="G12" s="49" t="n"/>
       <c r="H12" s="49" t="n"/>
       <c r="I12" s="48" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J12" s="48" t="inlineStr">
         <is>
-          <t>CTN</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K12" s="55" t="n"/>
@@ -1186,25 +1186,29 @@
       </c>
       <c r="B13" s="49" t="inlineStr">
         <is>
-          <t>SPONGE CLEANER 150X100X50MM</t>
+          <t>BULLDOZER, D6N, CATERPILLAR</t>
         </is>
       </c>
       <c r="C13" s="50" t="n"/>
       <c r="D13" s="51" t="n"/>
-      <c r="E13" s="49" t="n"/>
+      <c r="E13" s="49" t="inlineStr">
+        <is>
+          <t>CATERPILLAR 1123455</t>
+        </is>
+      </c>
       <c r="F13" s="49" t="inlineStr">
         <is>
-          <t>174058 IMPA MAKER: IMPA CATALOG</t>
+          <t>617130 BULLDOZER6N</t>
         </is>
       </c>
       <c r="G13" s="49" t="n"/>
       <c r="H13" s="49" t="n"/>
       <c r="I13" s="48" t="n">
-        <v>200</v>
+        <v>1</v>
       </c>
       <c r="J13" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K13" s="55" t="n"/>
@@ -1218,7 +1222,7 @@
       </c>
       <c r="B14" s="49" t="inlineStr">
         <is>
-          <t>STEEL WOOL NO.3 450GRM</t>
+          <t>JACKHAMMER, 30MM, ELECTRIC</t>
         </is>
       </c>
       <c r="C14" s="50" t="n"/>
@@ -1226,17 +1230,17 @@
       <c r="E14" s="49" t="n"/>
       <c r="F14" s="49" t="inlineStr">
         <is>
-          <t>174061 IMPA MAKER: IMPA CATALOG</t>
+          <t>617131 JACKHAMMER30</t>
         </is>
       </c>
       <c r="G14" s="49" t="n"/>
       <c r="H14" s="49" t="n"/>
       <c r="I14" s="48" t="n">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="J14" s="48" t="inlineStr">
         <is>
-          <t>PKT</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K14" s="55" t="n"/>
@@ -1250,7 +1254,7 @@
       </c>
       <c r="B15" s="49" t="inlineStr">
         <is>
-          <t>BRUSH DISHWASHING</t>
+          <t>AIR COMPRESSOR, 7.5HP, 200L TANK</t>
         </is>
       </c>
       <c r="C15" s="50" t="n"/>
@@ -1258,17 +1262,17 @@
       <c r="E15" s="49" t="n"/>
       <c r="F15" s="49" t="inlineStr">
         <is>
-          <t>174101 IMPA MAKER: IMPA CATALOG</t>
+          <t>617132 AIRCOMP200</t>
         </is>
       </c>
       <c r="G15" s="49" t="n"/>
       <c r="H15" s="49" t="n"/>
       <c r="I15" s="48" t="n">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="J15" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K15" s="55" t="n"/>
@@ -1282,7 +1286,7 @@
       </c>
       <c r="B16" s="49" t="inlineStr">
         <is>
-          <t>DUST PAN PLASTIC FLAT</t>
+          <t>CEMENT BAGS, 50KG</t>
         </is>
       </c>
       <c r="C16" s="50" t="n"/>
@@ -1290,17 +1294,17 @@
       <c r="E16" s="49" t="n"/>
       <c r="F16" s="49" t="inlineStr">
         <is>
-          <t>174141 IMPA MAKER: IMPA CATALOG</t>
+          <t>617133 CEMENT50</t>
         </is>
       </c>
       <c r="G16" s="49" t="n"/>
       <c r="H16" s="49" t="n"/>
       <c r="I16" s="48" t="n">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="J16" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>bags</t>
         </is>
       </c>
       <c r="K16" s="55" t="n"/>
@@ -1314,7 +1318,7 @@
       </c>
       <c r="B17" s="49" t="inlineStr">
         <is>
-          <t>PLASTIC BAG TRANSPARENT, 650X850MM 10S</t>
+          <t>STEEL REBAR, 12MM DIAMETER, 6M LENGTH</t>
         </is>
       </c>
       <c r="C17" s="50" t="n"/>
@@ -1322,17 +1326,17 @@
       <c r="E17" s="49" t="n"/>
       <c r="F17" s="49" t="inlineStr">
         <is>
-          <t>174174 IMPA MAKER: IMPA CATALOG</t>
+          <t>617134 REBAR12</t>
         </is>
       </c>
       <c r="G17" s="49" t="n"/>
       <c r="H17" s="49" t="n"/>
       <c r="I17" s="48" t="n">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="J17" s="48" t="inlineStr">
         <is>
-          <t>PKT</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K17" s="55" t="n"/>
@@ -1346,7 +1350,7 @@
       </c>
       <c r="B18" s="49" t="inlineStr">
         <is>
-          <t>PAPER TOWEL ROLLED 280MMX14M</t>
+          <t>SHOVELS, STAINLESS STEEL, 120CM</t>
         </is>
       </c>
       <c r="C18" s="50" t="n"/>
@@ -1354,17 +1358,17 @@
       <c r="E18" s="49" t="n"/>
       <c r="F18" s="49" t="inlineStr">
         <is>
-          <t>174232 IMPA MAKER: IMPA CATALOG</t>
+          <t>617135 SHOVEL120</t>
         </is>
       </c>
       <c r="G18" s="49" t="n"/>
       <c r="H18" s="49" t="n"/>
       <c r="I18" s="48" t="n">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="J18" s="48" t="inlineStr">
         <is>
-          <t>RLS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K18" s="55" t="n"/>
@@ -1378,7 +1382,7 @@
       </c>
       <c r="B19" s="49" t="inlineStr">
         <is>
-          <t>TOILET PAPER 2-PLY SOFT 100S</t>
+          <t>STEEL TROWELS, 180MM BLADE</t>
         </is>
       </c>
       <c r="C19" s="50" t="n"/>
@@ -1386,17 +1390,17 @@
       <c r="E19" s="49" t="n"/>
       <c r="F19" s="49" t="inlineStr">
         <is>
-          <t>174244 IMPA MAKER: IMPA CATALOG</t>
+          <t>617136 TROWEL180</t>
         </is>
       </c>
       <c r="G19" s="49" t="n"/>
       <c r="H19" s="49" t="n"/>
       <c r="I19" s="48" t="n">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="J19" s="48" t="inlineStr">
         <is>
-          <t>C/T</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K19" s="55" t="n"/>
@@ -1410,7 +1414,7 @@
       </c>
       <c r="B20" s="49" t="inlineStr">
         <is>
-          <t>SPRING CLAMP MOP</t>
+          <t>LEVELING INSTRUMENTS, LASER, 50M RANGE</t>
         </is>
       </c>
       <c r="C20" s="50" t="n"/>
@@ -1418,17 +1422,17 @@
       <c r="E20" s="49" t="n"/>
       <c r="F20" s="49" t="inlineStr">
         <is>
-          <t>174275 IMPA MAKER: IMPA CATALOG</t>
+          <t>617137 LEVEL50</t>
         </is>
       </c>
       <c r="G20" s="49" t="n"/>
       <c r="H20" s="49" t="n"/>
       <c r="I20" s="48" t="n">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="J20" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K20" s="55" t="n"/>
@@ -1442,7 +1446,7 @@
       </c>
       <c r="B21" s="49" t="inlineStr">
         <is>
-          <t>HEAD FOR SPRING CLAMP MOP</t>
+          <t>SCAFFOLDING COMPONENTS, ALUMINUM, 3M HEIGHT</t>
         </is>
       </c>
       <c r="C21" s="50" t="n"/>
@@ -1450,17 +1454,17 @@
       <c r="E21" s="49" t="n"/>
       <c r="F21" s="49" t="inlineStr">
         <is>
-          <t>174277 IMPA MAKER: IMPA CATALOG</t>
+          <t>617138 SCAFFOLD3M</t>
         </is>
       </c>
       <c r="G21" s="49" t="n"/>
       <c r="H21" s="49" t="n"/>
       <c r="I21" s="48" t="n">
-        <v>100</v>
+        <v>15</v>
       </c>
       <c r="J21" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K21" s="55" t="n"/>
@@ -1474,7 +1478,7 @@
       </c>
       <c r="B22" s="49" t="inlineStr">
         <is>
-          <t>WRINGER MOP BUCKET</t>
+          <t>WELDING MACHINE, MIG/TIG, 250A</t>
         </is>
       </c>
       <c r="C22" s="50" t="n"/>
@@ -1482,17 +1486,17 @@
       <c r="E22" s="49" t="n"/>
       <c r="F22" s="49" t="inlineStr">
         <is>
-          <t>174280 IMPA MAKER: IMPA CATALOG</t>
+          <t>617139 WELD250</t>
         </is>
       </c>
       <c r="G22" s="49" t="n"/>
       <c r="H22" s="49" t="n"/>
       <c r="I22" s="48" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="J22" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K22" s="55" t="n"/>
@@ -1506,7 +1510,7 @@
       </c>
       <c r="B23" s="49" t="inlineStr">
         <is>
-          <t>SAFETY MATCH 12S</t>
+          <t>INDUSTRIAL WELDING RODS, 2.5MM, 5KG BOX</t>
         </is>
       </c>
       <c r="C23" s="50" t="n"/>
@@ -1514,17 +1518,17 @@
       <c r="E23" s="49" t="n"/>
       <c r="F23" s="49" t="inlineStr">
         <is>
-          <t>174301 IMPA MAKER: IMPA CATALOG</t>
+          <t>617140 WELDROD2.5</t>
         </is>
       </c>
       <c r="G23" s="49" t="n"/>
       <c r="H23" s="49" t="n"/>
       <c r="I23" s="48" t="n">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="J23" s="48" t="inlineStr">
         <is>
-          <t>PKT</t>
+          <t>boxes</t>
         </is>
       </c>
       <c r="K23" s="55" t="n"/>
@@ -1538,7 +1542,7 @@
       </c>
       <c r="B24" s="49" t="inlineStr">
         <is>
-          <t>THERMO POT ELECTRIC, 3.8LTR 220V</t>
+          <t>ANGLE GRINDER, 125MM, CORDLESS</t>
         </is>
       </c>
       <c r="C24" s="50" t="n"/>
@@ -1546,17 +1550,17 @@
       <c r="E24" s="49" t="n"/>
       <c r="F24" s="49" t="inlineStr">
         <is>
-          <t>174529 IMPA MAKER: IMPA CATALOG</t>
+          <t>617141 ANGLEGRIND125</t>
         </is>
       </c>
       <c r="G24" s="49" t="n"/>
       <c r="H24" s="49" t="n"/>
       <c r="I24" s="48" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J24" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K24" s="55" t="n"/>
@@ -1570,7 +1574,7 @@
       </c>
       <c r="B25" s="49" t="inlineStr">
         <is>
-          <t>GLOVES WORKING COTTON ORDINARY</t>
+          <t>CIRCULAR SAW, 235MM BLADE, 1800W</t>
         </is>
       </c>
       <c r="C25" s="50" t="n"/>
@@ -1578,17 +1582,17 @@
       <c r="E25" s="49" t="n"/>
       <c r="F25" s="49" t="inlineStr">
         <is>
-          <t>190104 IMPA MAKER: IMPA CATALOG</t>
+          <t>617142 CIRCULARSAW235</t>
         </is>
       </c>
       <c r="G25" s="49" t="n"/>
       <c r="H25" s="49" t="n"/>
       <c r="I25" s="48" t="n">
-        <v>300</v>
+        <v>3</v>
       </c>
       <c r="J25" s="48" t="inlineStr">
         <is>
-          <t>PRS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K25" s="55" t="n"/>
@@ -1602,7 +1606,7 @@
       </c>
       <c r="B26" s="49" t="inlineStr">
         <is>
-          <t>GLOVES WORKING COTTON, RUBBER COATED PALM</t>
+          <t>JIGSAW, 650W, VARIABLE SPEED</t>
         </is>
       </c>
       <c r="C26" s="50" t="n"/>
@@ -1610,17 +1614,17 @@
       <c r="E26" s="49" t="n"/>
       <c r="F26" s="49" t="inlineStr">
         <is>
-          <t>190102 IMPA MAKER: IMPA CATALOG</t>
+          <t>617143 JIGSAW650</t>
         </is>
       </c>
       <c r="G26" s="49" t="n"/>
       <c r="H26" s="49" t="n"/>
       <c r="I26" s="48" t="n">
-        <v>300</v>
+        <v>2</v>
       </c>
       <c r="J26" s="48" t="inlineStr">
         <is>
-          <t>PRS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K26" s="55" t="n"/>
@@ -1634,7 +1638,7 @@
       </c>
       <c r="B27" s="49" t="inlineStr">
         <is>
-          <t>GLOVES WINTER VINYL LEATHER, SIZE:L</t>
+          <t>HAMMER, 1KG, WOODEN HANDLE</t>
         </is>
       </c>
       <c r="C27" s="50" t="n"/>
@@ -1642,17 +1646,17 @@
       <c r="E27" s="49" t="n"/>
       <c r="F27" s="49" t="inlineStr">
         <is>
-          <t>190107 IMPA MAKER: IMPA CATALOG</t>
+          <t>617144 HAMMER1KG</t>
         </is>
       </c>
       <c r="G27" s="49" t="n"/>
       <c r="H27" s="49" t="n"/>
       <c r="I27" s="48" t="n">
-        <v>200</v>
+        <v>10</v>
       </c>
       <c r="J27" s="48" t="inlineStr">
         <is>
-          <t>PRS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K27" s="55" t="n"/>
@@ -1666,7 +1670,7 @@
       </c>
       <c r="B28" s="49" t="inlineStr">
         <is>
-          <t>GLOVES PLASTIC OIL/ACID RESIST, LONG</t>
+          <t>TAPE MEASURE, 100M, FIBERGLASS</t>
         </is>
       </c>
       <c r="C28" s="50" t="n"/>
@@ -1674,17 +1678,17 @@
       <c r="E28" s="49" t="n"/>
       <c r="F28" s="49" t="inlineStr">
         <is>
-          <t>190132 IMPA MAKER: IMPA CATALOG</t>
+          <t>617145 TAPEMEASURE100</t>
         </is>
       </c>
       <c r="G28" s="49" t="n"/>
       <c r="H28" s="49" t="n"/>
       <c r="I28" s="48" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="J28" s="48" t="inlineStr">
         <is>
-          <t>PRS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K28" s="55" t="n"/>
@@ -1698,7 +1702,7 @@
       </c>
       <c r="B29" s="49" t="inlineStr">
         <is>
-          <t>CAP BASEBALL TYPE COTTON</t>
+          <t>LASER LEVEL, SELF-LEVELING, 30M RANGE</t>
         </is>
       </c>
       <c r="C29" s="50" t="n"/>
@@ -1706,17 +1710,17 @@
       <c r="E29" s="49" t="n"/>
       <c r="F29" s="49" t="inlineStr">
         <is>
-          <t>190476 IMPA MAKER: IMPA CATALOG</t>
+          <t>617146 LASERLEVEL30</t>
         </is>
       </c>
       <c r="G29" s="49" t="n"/>
       <c r="H29" s="49" t="n"/>
       <c r="I29" s="48" t="n">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="J29" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K29" s="55" t="n"/>
@@ -1730,7 +1734,7 @@
       </c>
       <c r="B30" s="49" t="inlineStr">
         <is>
-          <t>CAP WINTER KNIT POINTED CROWN</t>
+          <t>CONCRETE VIBRATOR, 1.5KW, 3M HOSE</t>
         </is>
       </c>
       <c r="C30" s="50" t="n"/>
@@ -1738,17 +1742,17 @@
       <c r="E30" s="49" t="n"/>
       <c r="F30" s="49" t="inlineStr">
         <is>
-          <t>190631 IMPA MAKER: IMPA CATALOG</t>
+          <t>617147 CONCRETEVIB1.5</t>
         </is>
       </c>
       <c r="G30" s="49" t="n"/>
       <c r="H30" s="49" t="n"/>
       <c r="I30" s="48" t="n">
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="J30" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K30" s="55" t="n"/>
@@ -1762,7 +1766,7 @@
       </c>
       <c r="B31" s="49" t="inlineStr">
         <is>
-          <t>HEAVING LINE POLYPROPYLENE, 1IN CIR X 200M</t>
+          <t>WHEELBARROWS, STEEL, 100L CAPACITY</t>
         </is>
       </c>
       <c r="C31" s="50" t="n"/>
@@ -1770,17 +1774,17 @@
       <c r="E31" s="49" t="n"/>
       <c r="F31" s="49" t="inlineStr">
         <is>
-          <t>211271 IMPA MAKER: IMPA CATALOG</t>
+          <t>617148 WHEELBARROW100</t>
         </is>
       </c>
       <c r="G31" s="49" t="n"/>
       <c r="H31" s="49" t="n"/>
       <c r="I31" s="48" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J31" s="48" t="inlineStr">
         <is>
-          <t>C/L</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K31" s="55" t="n"/>
@@ -1794,7 +1798,7 @@
       </c>
       <c r="B32" s="49" t="inlineStr">
         <is>
-          <t>HEAVING LINE POLYPROPYLENE, 1-1/4IN CIR X 200M</t>
+          <t>LADDERS, ALUMINUM, 3-STEP, 2M HEIGHT</t>
         </is>
       </c>
       <c r="C32" s="50" t="n"/>
@@ -1802,17 +1806,17 @@
       <c r="E32" s="49" t="n"/>
       <c r="F32" s="49" t="inlineStr">
         <is>
-          <t>211273 IMPA MAKER: IMPA CATALOG</t>
+          <t>617149 LADDER3STEP</t>
         </is>
       </c>
       <c r="G32" s="49" t="n"/>
       <c r="H32" s="49" t="n"/>
       <c r="I32" s="48" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J32" s="48" t="inlineStr">
         <is>
-          <t>C/L</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K32" s="55" t="n"/>
@@ -1826,7 +1830,7 @@
       </c>
       <c r="B33" s="49" t="inlineStr">
         <is>
-          <t>TIGERROPE POLYETHYLENE 3STRAND, BLACK/YELLOW 1IN CIRX200M</t>
+          <t>SAFETY HELMETS, POLYETHYLENE, SIZE M/L</t>
         </is>
       </c>
       <c r="C33" s="50" t="n"/>
@@ -1834,17 +1838,17 @@
       <c r="E33" s="49" t="n"/>
       <c r="F33" s="49" t="inlineStr">
         <is>
-          <t>211352 IMPA MAKER: IMPA CATALOG</t>
+          <t>617150 HELMETSIZEM</t>
         </is>
       </c>
       <c r="G33" s="49" t="n"/>
       <c r="H33" s="49" t="n"/>
       <c r="I33" s="48" t="n">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="J33" s="48" t="inlineStr">
         <is>
-          <t>C/L</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K33" s="55" t="n"/>
@@ -1858,7 +1862,7 @@
       </c>
       <c r="B34" s="49" t="inlineStr">
         <is>
-          <t>SLING BELT POLYESTER, WIDTH 50MM X L 4M</t>
+          <t>SAFETY GLOVES, NITRILE, MEDIUM</t>
         </is>
       </c>
       <c r="C34" s="50" t="n"/>
@@ -1866,17 +1870,17 @@
       <c r="E34" s="49" t="n"/>
       <c r="F34" s="49" t="inlineStr">
         <is>
-          <t>232146 IMPA MAKER: IMPA CATALOG</t>
+          <t>617151 GLOVENITRILE</t>
         </is>
       </c>
       <c r="G34" s="49" t="n"/>
       <c r="H34" s="49" t="n"/>
       <c r="I34" s="48" t="n">
-        <v>2</v>
+        <v>100</v>
       </c>
       <c r="J34" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K34" s="55" t="n"/>
@@ -1890,7 +1894,7 @@
       </c>
       <c r="B35" s="49" t="inlineStr">
         <is>
-          <t>SLING BELT POLYESTER, WIDTH 75MM X L 5M</t>
+          <t>WORK BOOTS, STEEL TOE, SIZE 42</t>
         </is>
       </c>
       <c r="C35" s="50" t="n"/>
@@ -1898,17 +1902,17 @@
       <c r="E35" s="49" t="n"/>
       <c r="F35" s="49" t="inlineStr">
         <is>
-          <t>232175 IMPA MAKER: IMPA CATALOG</t>
+          <t>617152 BOOTSTEEL42</t>
         </is>
       </c>
       <c r="G35" s="49" t="n"/>
       <c r="H35" s="49" t="n"/>
       <c r="I35" s="48" t="n">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="J35" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K35" s="55" t="n"/>
@@ -1922,7 +1926,7 @@
       </c>
       <c r="B36" s="49" t="inlineStr">
         <is>
-          <t>SCUPPER PLUG 110MM PLUG DIAM</t>
+          <t>RESPIRATOR MASKS, N95, 10-PACK</t>
         </is>
       </c>
       <c r="C36" s="50" t="n"/>
@@ -1930,17 +1934,17 @@
       <c r="E36" s="49" t="n"/>
       <c r="F36" s="49" t="inlineStr">
         <is>
-          <t>232486 IMPA MAKER: IMPA CATALOG</t>
+          <t>617153 RESPIRATORN95</t>
         </is>
       </c>
       <c r="G36" s="49" t="n"/>
       <c r="H36" s="49" t="n"/>
       <c r="I36" s="48" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="J36" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>packs</t>
         </is>
       </c>
       <c r="K36" s="55" t="n"/>
@@ -1954,7 +1958,7 @@
       </c>
       <c r="B37" s="49" t="inlineStr">
         <is>
-          <t>SCUPPER PLUG 135MM PLUG DIAM</t>
+          <t>HIGH-VISIBILITY JACKETS, POLYESTER, SIZE L</t>
         </is>
       </c>
       <c r="C37" s="50" t="n"/>
@@ -1962,17 +1966,17 @@
       <c r="E37" s="49" t="n"/>
       <c r="F37" s="49" t="inlineStr">
         <is>
-          <t>232487 IMPA MAKER: IMPA CATALOG</t>
+          <t>617154 VESTHIGHVISL</t>
         </is>
       </c>
       <c r="G37" s="49" t="n"/>
       <c r="H37" s="49" t="n"/>
       <c r="I37" s="48" t="n">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="J37" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K37" s="55" t="n"/>
@@ -1986,7 +1990,7 @@
       </c>
       <c r="B38" s="49" t="inlineStr">
         <is>
-          <t>WASTE COTTON STERILIZED WHITE</t>
+          <t>STEEL BEAMS, I-BEAM, 150MM</t>
         </is>
       </c>
       <c r="C38" s="50" t="n"/>
@@ -1994,17 +1998,17 @@
       <c r="E38" s="49" t="n"/>
       <c r="F38" s="49" t="inlineStr">
         <is>
-          <t>232901 IMPA MAKER: IMPA CATALOG</t>
+          <t>617155 BEAM150</t>
         </is>
       </c>
       <c r="G38" s="49" t="n"/>
       <c r="H38" s="49" t="n"/>
       <c r="I38" s="48" t="n">
-        <v>200</v>
+        <v>10</v>
       </c>
       <c r="J38" s="48" t="inlineStr">
         <is>
-          <t>KGS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K38" s="55" t="n"/>
@@ -2018,7 +2022,7 @@
       </c>
       <c r="B39" s="49" t="inlineStr">
         <is>
-          <t>FIRE AXE WITH WOOD HANDLE</t>
+          <t>LUMBER, PINEWOOD, 2X4, 3M LENGTH</t>
         </is>
       </c>
       <c r="C39" s="50" t="n"/>
@@ -2026,17 +2030,17 @@
       <c r="E39" s="49" t="n"/>
       <c r="F39" s="49" t="inlineStr">
         <is>
-          <t>330961 IMPA MAKER: IMPA CATALOG</t>
+          <t>617156 LUMBER2X4</t>
         </is>
       </c>
       <c r="G39" s="49" t="n"/>
       <c r="H39" s="49" t="n"/>
       <c r="I39" s="48" t="n">
-        <v>3</v>
+        <v>50</v>
       </c>
       <c r="J39" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K39" s="55" t="n"/>
@@ -2050,7 +2054,7 @@
       </c>
       <c r="B40" s="49" t="inlineStr">
         <is>
-          <t>SPARE SHIELD POLYCARBONATE FOR,SPARE SHIELD POLYCARBONATE</t>
+          <t>PLYWOOD SHEETS, 18MM THICK, 2400X1200MM</t>
         </is>
       </c>
       <c r="C40" s="50" t="n"/>
@@ -2058,17 +2062,17 @@
       <c r="E40" s="49" t="n"/>
       <c r="F40" s="49" t="inlineStr">
         <is>
-          <t>331148 IMPA MAKER: IMPA CATALOG</t>
+          <t>617157 PLYWOOD18</t>
         </is>
       </c>
       <c r="G40" s="49" t="n"/>
       <c r="H40" s="49" t="n"/>
       <c r="I40" s="48" t="n">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="J40" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K40" s="55" t="n"/>
@@ -2082,7 +2086,7 @@
       </c>
       <c r="B41" s="49" t="inlineStr">
         <is>
-          <t>LUBRICANT WD-40 SPRAY 360ML</t>
+          <t>METAL SHEETS, GALVANIZED STEEL, 1MM THICK</t>
         </is>
       </c>
       <c r="C41" s="50" t="n"/>
@@ -2090,7 +2094,7 @@
       <c r="E41" s="49" t="n"/>
       <c r="F41" s="49" t="inlineStr">
         <is>
-          <t>450702 IMPA MAKER: IMPA CATALOG</t>
+          <t>617158 METALSHEET1</t>
         </is>
       </c>
       <c r="G41" s="49" t="n"/>
@@ -2100,7 +2104,7 @@
       </c>
       <c r="J41" s="48" t="inlineStr">
         <is>
-          <t>TIN</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K41" s="55" t="n"/>
@@ -2114,7 +2118,7 @@
       </c>
       <c r="B42" s="49" t="inlineStr">
         <is>
-          <t>TAPE MASKING PAPER 48MMXL55M</t>
+          <t>INSULATION MATERIAL, ROCK WOOL, 50MM THICK</t>
         </is>
       </c>
       <c r="C42" s="50" t="n"/>
@@ -2122,17 +2126,17 @@
       <c r="E42" s="49" t="n"/>
       <c r="F42" s="49" t="inlineStr">
         <is>
-          <t>471378 IMPA MAKER: IMPA CATALOG</t>
+          <t>617159 INSULATION50</t>
         </is>
       </c>
       <c r="G42" s="49" t="n"/>
       <c r="H42" s="49" t="n"/>
       <c r="I42" s="48" t="n">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="J42" s="48" t="inlineStr">
         <is>
-          <t>RLS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K42" s="55" t="n"/>
@@ -2146,7 +2150,7 @@
       </c>
       <c r="B43" s="49" t="inlineStr">
         <is>
-          <t>PADLOCK BRASS 50MM WITH 2KEYS</t>
+          <t>ROOFING MATERIALS, ASPHALT SHINGLES, 1.2X0.3M</t>
         </is>
       </c>
       <c r="C43" s="50" t="n"/>
@@ -2154,17 +2158,17 @@
       <c r="E43" s="49" t="n"/>
       <c r="F43" s="49" t="inlineStr">
         <is>
-          <t>490505 IMPA MAKER: IMPA CATALOG</t>
+          <t>617160 SHINGLES120</t>
         </is>
       </c>
       <c r="G43" s="49" t="n"/>
       <c r="H43" s="49" t="n"/>
       <c r="I43" s="48" t="n">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="J43" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K43" s="55" t="n"/>
@@ -2178,7 +2182,7 @@
       </c>
       <c r="B44" s="49" t="inlineStr">
         <is>
-          <t>DOOR CLOSER STANDARD, MAXIMUM DOOR WEIGHT 65KGS</t>
+          <t>BRICKS, CLAY, 250X120X65MM</t>
         </is>
       </c>
       <c r="C44" s="50" t="n"/>
@@ -2186,17 +2190,17 @@
       <c r="E44" s="49" t="n"/>
       <c r="F44" s="49" t="inlineStr">
         <is>
-          <t>490603 IMPA MAKER: IMPA CATALOG</t>
+          <t>617161 CLAYBRICK250</t>
         </is>
       </c>
       <c r="G44" s="49" t="n"/>
       <c r="H44" s="49" t="n"/>
       <c r="I44" s="48" t="n">
-        <v>5</v>
+        <v>1000</v>
       </c>
       <c r="J44" s="48" t="inlineStr">
         <is>
-          <t>SET</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K44" s="55" t="n"/>
@@ -2210,7 +2214,7 @@
       </c>
       <c r="B45" s="49" t="inlineStr">
         <is>
-          <t>DOOR CLOSER STANDARD, MAXIMUM DOOR WEIGHT 85KGS</t>
+          <t>MORTAR MIX, CEMENT BASED, 25KG BAG</t>
         </is>
       </c>
       <c r="C45" s="50" t="n"/>
@@ -2218,17 +2222,17 @@
       <c r="E45" s="49" t="n"/>
       <c r="F45" s="49" t="inlineStr">
         <is>
-          <t>490604 IMPA MAKER: IMPA CATALOG</t>
+          <t>617162 MORTARMIX25</t>
         </is>
       </c>
       <c r="G45" s="49" t="n"/>
       <c r="H45" s="49" t="n"/>
       <c r="I45" s="48" t="n">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="J45" s="48" t="inlineStr">
         <is>
-          <t>SET</t>
+          <t>bags</t>
         </is>
       </c>
       <c r="K45" s="55" t="n"/>
@@ -2242,7 +2246,7 @@
       </c>
       <c r="B46" s="49" t="inlineStr">
         <is>
-          <t>BRUSH RADIATOR ANGLE(DOG LEG), 50MM WIDTH</t>
+          <t>SAND, CONSTRUCTION GRADE, 1M³</t>
         </is>
       </c>
       <c r="C46" s="50" t="n"/>
@@ -2250,17 +2254,17 @@
       <c r="E46" s="49" t="n"/>
       <c r="F46" s="49" t="inlineStr">
         <is>
-          <t>510167 IMPA MAKER: IMPA CATALOG</t>
+          <t>617163 SANDGRADE1M3</t>
         </is>
       </c>
       <c r="G46" s="49" t="n"/>
       <c r="H46" s="49" t="n"/>
       <c r="I46" s="48" t="n">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="J46" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>m³</t>
         </is>
       </c>
       <c r="K46" s="55" t="n"/>
@@ -2274,7 +2278,7 @@
       </c>
       <c r="B47" s="49" t="inlineStr">
         <is>
-          <t>BRUSH RADIATOR ANGLE(DOG LEG), 65MM WIDTH</t>
+          <t>GRAVEL, 20MM, 1M³</t>
         </is>
       </c>
       <c r="C47" s="50" t="n"/>
@@ -2282,17 +2286,17 @@
       <c r="E47" s="49" t="n"/>
       <c r="F47" s="49" t="inlineStr">
         <is>
-          <t>510168 IMPA MAKER: IMPA CATALOG</t>
+          <t>617164 GRAVEL20MM</t>
         </is>
       </c>
       <c r="G47" s="49" t="n"/>
       <c r="H47" s="49" t="n"/>
       <c r="I47" s="48" t="n">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="J47" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>m³</t>
         </is>
       </c>
       <c r="K47" s="55" t="n"/>
@@ -2306,7 +2310,7 @@
       </c>
       <c r="B48" s="49" t="inlineStr">
         <is>
-          <t>BRUSH PAINT ROLLER MINI, WITH HANDLE 100MM WIDTH</t>
+          <t>CEMENT BAGS, 25KG</t>
         </is>
       </c>
       <c r="C48" s="50" t="n"/>
@@ -2314,17 +2318,17 @@
       <c r="E48" s="49" t="n"/>
       <c r="F48" s="49" t="inlineStr">
         <is>
-          <t>510461 IMPA MAKER: IMPA CATALOG</t>
+          <t>617165 CEMENT25</t>
         </is>
       </c>
       <c r="G48" s="49" t="n"/>
       <c r="H48" s="49" t="n"/>
       <c r="I48" s="48" t="n">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="J48" s="48" t="inlineStr">
         <is>
-          <t>SET</t>
+          <t>bags</t>
         </is>
       </c>
       <c r="K48" s="55" t="n"/>
@@ -2338,7 +2342,7 @@
       </c>
       <c r="B49" s="49" t="inlineStr">
         <is>
-          <t>SPARE MINI ROLLER 100MM WIDTH</t>
+          <t>STONE DUST, 1M³</t>
         </is>
       </c>
       <c r="C49" s="50" t="n"/>
@@ -2346,17 +2350,17 @@
       <c r="E49" s="49" t="n"/>
       <c r="F49" s="49" t="inlineStr">
         <is>
-          <t>510462 IMPA MAKER: IMPA CATALOG</t>
+          <t>617166 STONEDUST1M3</t>
         </is>
       </c>
       <c r="G49" s="49" t="n"/>
       <c r="H49" s="49" t="n"/>
       <c r="I49" s="48" t="n">
-        <v>500</v>
+        <v>15</v>
       </c>
       <c r="J49" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>m³</t>
         </is>
       </c>
       <c r="K49" s="55" t="n"/>
@@ -2370,7 +2374,7 @@
       </c>
       <c r="B50" s="49" t="inlineStr">
         <is>
-          <t>BRUSH DECK NYLON HEAD ONLY, 180MM WIDTH</t>
+          <t>CONSTRUCTION PAINT, EXTERIOR, 20L</t>
         </is>
       </c>
       <c r="C50" s="50" t="n"/>
@@ -2378,7 +2382,7 @@
       <c r="E50" s="49" t="n"/>
       <c r="F50" s="49" t="inlineStr">
         <is>
-          <t>510612 IMPA MAKER: IMPA CATALOG</t>
+          <t>617167 PAINTEXTERIOR</t>
         </is>
       </c>
       <c r="G50" s="49" t="n"/>
@@ -2388,7 +2392,7 @@
       </c>
       <c r="J50" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K50" s="55" t="n"/>
@@ -2402,7 +2406,7 @@
       </c>
       <c r="B51" s="49" t="inlineStr">
         <is>
-          <t>BRUSH SWEEPING SOFT BRISTLE, HEAD ONLY W200MM</t>
+          <t>PAINT BRUSHES, 2” AND 4”</t>
         </is>
       </c>
       <c r="C51" s="50" t="n"/>
@@ -2410,17 +2414,17 @@
       <c r="E51" s="49" t="n"/>
       <c r="F51" s="49" t="inlineStr">
         <is>
-          <t>510622 IMPA MAKER: IMPA CATALOG</t>
+          <t>617168 PAINTBRUSHES</t>
         </is>
       </c>
       <c r="G51" s="49" t="n"/>
       <c r="H51" s="49" t="n"/>
       <c r="I51" s="48" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="J51" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K51" s="55" t="n"/>
@@ -2434,7 +2438,7 @@
       </c>
       <c r="B52" s="49" t="inlineStr">
         <is>
-          <t>BRUSH HAND SCRUB WHITE HAIR, SQUARE</t>
+          <t>PAINT ROLLERS, 9”</t>
         </is>
       </c>
       <c r="C52" s="50" t="n"/>
@@ -2442,7 +2446,7 @@
       <c r="E52" s="49" t="n"/>
       <c r="F52" s="49" t="inlineStr">
         <is>
-          <t>510652 IMPA MAKER: IMPA CATALOG</t>
+          <t>617169 PAINTROLLER9</t>
         </is>
       </c>
       <c r="G52" s="49" t="n"/>
@@ -2452,7 +2456,7 @@
       </c>
       <c r="J52" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K52" s="55" t="n"/>
@@ -2466,7 +2470,7 @@
       </c>
       <c r="B53" s="49" t="inlineStr">
         <is>
-          <t>MAT BATH &amp; SHOWER RUBBER, SAFE FOOTING 355X558MM</t>
+          <t>CAULKING GUN, STEEL, 10-12 OZ CARTRIDGE</t>
         </is>
       </c>
       <c r="C53" s="50" t="n"/>
@@ -2474,17 +2478,17 @@
       <c r="E53" s="49" t="n"/>
       <c r="F53" s="49" t="inlineStr">
         <is>
-          <t>511010 IMPA MAKER: IMPA CATALOG</t>
+          <t>617170 CAULKINGGUN</t>
         </is>
       </c>
       <c r="G53" s="49" t="n"/>
       <c r="H53" s="49" t="n"/>
       <c r="I53" s="48" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="J53" s="48" t="inlineStr">
         <is>
-          <t>SHT</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K53" s="55" t="n"/>
@@ -2498,7 +2502,7 @@
       </c>
       <c r="B54" s="49" t="inlineStr">
         <is>
-          <t>MAT DOOR VINYL(KARAKUSA), 45X75CM</t>
+          <t>CONCRETE FORMS, WOODEN, 2M LENGTH</t>
         </is>
       </c>
       <c r="C54" s="50" t="n"/>
@@ -2506,17 +2510,17 @@
       <c r="E54" s="49" t="n"/>
       <c r="F54" s="49" t="inlineStr">
         <is>
-          <t>511037 IMPA MAKER: IMPA CATALOG</t>
+          <t>617171 CONCRETEFORM2M</t>
         </is>
       </c>
       <c r="G54" s="49" t="n"/>
       <c r="H54" s="49" t="n"/>
       <c r="I54" s="48" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="J54" s="48" t="inlineStr">
         <is>
-          <t>SHT</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K54" s="55" t="n"/>
@@ -2530,7 +2534,7 @@
       </c>
       <c r="B55" s="49" t="inlineStr">
         <is>
-          <t>MAT DOOR VINYL(KARAKUSA), 60X90CM</t>
+          <t>CONCRETE RELEASE AGENT, 5L</t>
         </is>
       </c>
       <c r="C55" s="50" t="n"/>
@@ -2538,7 +2542,7 @@
       <c r="E55" s="49" t="n"/>
       <c r="F55" s="49" t="inlineStr">
         <is>
-          <t>511038 IMPA MAKER: IMPA CATALOG</t>
+          <t>617172 CONCRETELRELEASE</t>
         </is>
       </c>
       <c r="G55" s="49" t="n"/>
@@ -2548,7 +2552,7 @@
       </c>
       <c r="J55" s="48" t="inlineStr">
         <is>
-          <t>SHT</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K55" s="55" t="n"/>
@@ -2562,7 +2566,7 @@
       </c>
       <c r="B56" s="49" t="inlineStr">
         <is>
-          <t>DETERGENT LAUNDRY MACHINE, LIVETT 20KGS</t>
+          <t>REBAR TYING TOOL, MANUAL</t>
         </is>
       </c>
       <c r="C56" s="50" t="n"/>
@@ -2570,17 +2574,17 @@
       <c r="E56" s="49" t="n"/>
       <c r="F56" s="49" t="inlineStr">
         <is>
-          <t>550134 IMPA MAKER: IMPA CATALOG</t>
+          <t>617173 REBARTYING</t>
         </is>
       </c>
       <c r="G56" s="49" t="n"/>
       <c r="H56" s="49" t="n"/>
       <c r="I56" s="48" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="J56" s="48" t="inlineStr">
         <is>
-          <t>BAG</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K56" s="55" t="n"/>
@@ -2594,7 +2598,7 @@
       </c>
       <c r="B57" s="49" t="inlineStr">
         <is>
-          <t>CLEANER LIQUID KITCHEN H. DUTY, SPRAY 400ML</t>
+          <t>HYDRAULIC JACKS, 10 TON</t>
         </is>
       </c>
       <c r="C57" s="50" t="n"/>
@@ -2602,17 +2606,17 @@
       <c r="E57" s="49" t="n"/>
       <c r="F57" s="49" t="inlineStr">
         <is>
-          <t>550173 IMPA MAKER: IMPA CATALOG</t>
+          <t>617174 JACK10TON</t>
         </is>
       </c>
       <c r="G57" s="49" t="n"/>
       <c r="H57" s="49" t="n"/>
       <c r="I57" s="48" t="n">
-        <v>36</v>
+        <v>2</v>
       </c>
       <c r="J57" s="48" t="inlineStr">
         <is>
-          <t>BTL</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K57" s="55" t="n"/>
@@ -2626,7 +2630,7 @@
       </c>
       <c r="B58" s="49" t="inlineStr">
         <is>
-          <t>CLEANER BATHROOM SPRAY TYPE, 400ML</t>
+          <t>ADJUSTABLE WRENCH, 10”</t>
         </is>
       </c>
       <c r="C58" s="50" t="n"/>
@@ -2634,17 +2638,17 @@
       <c r="E58" s="49" t="n"/>
       <c r="F58" s="49" t="inlineStr">
         <is>
-          <t>550177 IMPA MAKER: IMPA CATALOG</t>
+          <t>617175 WRENCH10</t>
         </is>
       </c>
       <c r="G58" s="49" t="n"/>
       <c r="H58" s="49" t="n"/>
       <c r="I58" s="48" t="n">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="J58" s="48" t="inlineStr">
         <is>
-          <t>BTL</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K58" s="55" t="n"/>
@@ -2658,7 +2662,7 @@
       </c>
       <c r="B59" s="49" t="inlineStr">
         <is>
-          <t>CLEANER OVEN 300GRM</t>
+          <t>PIPE WRENCHES, 18”</t>
         </is>
       </c>
       <c r="C59" s="50" t="n"/>
@@ -2666,17 +2670,17 @@
       <c r="E59" s="49" t="n"/>
       <c r="F59" s="49" t="inlineStr">
         <is>
-          <t>550301 IMPA MAKER: IMPA CATALOG</t>
+          <t>617176 PIPEWRENCH18</t>
         </is>
       </c>
       <c r="G59" s="49" t="n"/>
       <c r="H59" s="49" t="n"/>
       <c r="I59" s="48" t="n">
-        <v>36</v>
+        <v>5</v>
       </c>
       <c r="J59" s="48" t="inlineStr">
         <is>
-          <t>TIN</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K59" s="55" t="n"/>
@@ -2690,7 +2694,7 @@
       </c>
       <c r="B60" s="49" t="inlineStr">
         <is>
-          <t>SOAP TOILET LUX 100GRMX72S</t>
+          <t>PLUMBING PIPES, PVC, 40MM</t>
         </is>
       </c>
       <c r="C60" s="50" t="n"/>
@@ -2698,17 +2702,17 @@
       <c r="E60" s="49" t="n"/>
       <c r="F60" s="49" t="inlineStr">
         <is>
-          <t>550253 IMPA MAKER: IMPA CATALOG</t>
+          <t>617177 PIPES40MM</t>
         </is>
       </c>
       <c r="G60" s="49" t="n"/>
       <c r="H60" s="49" t="n"/>
       <c r="I60" s="48" t="n">
-        <v>7</v>
+        <v>100</v>
       </c>
       <c r="J60" s="48" t="inlineStr">
         <is>
-          <t>C/T</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K60" s="55" t="n"/>
@@ -2722,7 +2726,7 @@
       </c>
       <c r="B61" s="49" t="inlineStr">
         <is>
-          <t>AIR FRESHENER 300ML</t>
+          <t>PIPE FITTINGS, COPPER, ELBOW 40MM</t>
         </is>
       </c>
       <c r="C61" s="50" t="n"/>
@@ -2730,17 +2734,17 @@
       <c r="E61" s="49" t="n"/>
       <c r="F61" s="49" t="inlineStr">
         <is>
-          <t>550331 IMPA MAKER: IMPA CATALOG</t>
+          <t>617178 FITTINGCOPPER40</t>
         </is>
       </c>
       <c r="G61" s="49" t="n"/>
       <c r="H61" s="49" t="n"/>
       <c r="I61" s="48" t="n">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="J61" s="48" t="inlineStr">
         <is>
-          <t>TIN</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K61" s="55" t="n"/>
@@ -2754,7 +2758,7 @@
       </c>
       <c r="B62" s="49" t="inlineStr">
         <is>
-          <t>LAUNDRY SOFTENER 1.65LTR</t>
+          <t>VALVES, GATE, 40MM</t>
         </is>
       </c>
       <c r="C62" s="50" t="n"/>
@@ -2762,17 +2766,17 @@
       <c r="E62" s="49" t="n"/>
       <c r="F62" s="49" t="inlineStr">
         <is>
-          <t>550124 IMPA MAKER: IMPA CATALOG</t>
+          <t>617179 VALVE40MM</t>
         </is>
       </c>
       <c r="G62" s="49" t="n"/>
       <c r="H62" s="49" t="n"/>
       <c r="I62" s="48" t="n">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="J62" s="48" t="inlineStr">
         <is>
-          <t>BTL</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K62" s="55" t="n"/>
@@ -2786,7 +2790,7 @@
       </c>
       <c r="B63" s="49" t="inlineStr">
         <is>
-          <t>DISPENSER FOR SWARFEGA 4KGS</t>
+          <t>PIPING INSULATION, FOAM, 1M LENGTH</t>
         </is>
       </c>
       <c r="C63" s="50" t="n"/>
@@ -2794,17 +2798,17 @@
       <c r="E63" s="49" t="n"/>
       <c r="F63" s="49" t="inlineStr">
         <is>
-          <t>550269 IMPA MAKER: IMPA CATALOG</t>
+          <t>617180 PIPEFOAM1M</t>
         </is>
       </c>
       <c r="G63" s="49" t="n"/>
       <c r="H63" s="49" t="n"/>
       <c r="I63" s="48" t="n">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="J63" s="48" t="inlineStr">
         <is>
-          <t>SET</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K63" s="55" t="n"/>
@@ -2818,7 +2822,7 @@
       </c>
       <c r="B64" s="49" t="inlineStr">
         <is>
-          <t>DERUSTING BRUSH AIR MAG9000, HOLGER CLASEN 9000MIN-1</t>
+          <t>PVC GLUE, 500ML</t>
         </is>
       </c>
       <c r="C64" s="50" t="n"/>
@@ -2826,17 +2830,17 @@
       <c r="E64" s="49" t="n"/>
       <c r="F64" s="49" t="inlineStr">
         <is>
-          <t>592071 IMPA MAKER: IMPA CATALOG</t>
+          <t>617181 PVCGLUE500</t>
         </is>
       </c>
       <c r="G64" s="49" t="n"/>
       <c r="H64" s="49" t="n"/>
       <c r="I64" s="48" t="n">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="J64" s="48" t="inlineStr">
         <is>
-          <t>SET</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K64" s="55" t="n"/>
@@ -2850,7 +2854,7 @@
       </c>
       <c r="B65" s="49" t="inlineStr">
         <is>
-          <t>BRUSH WIRE CUP PLAITED 60MMDIA, FOR DERUSTING BRUSH MAG9000</t>
+          <t>DRYWALL SHEETS, 12.5MM THICK, 2400X1200MM</t>
         </is>
       </c>
       <c r="C65" s="50" t="n"/>
@@ -2858,17 +2862,17 @@
       <c r="E65" s="49" t="n"/>
       <c r="F65" s="49" t="inlineStr">
         <is>
-          <t>592075 IMPA MAKER: IMPA CATALOG</t>
+          <t>617182 DRYWALL12MM</t>
         </is>
       </c>
       <c r="G65" s="49" t="n"/>
       <c r="H65" s="49" t="n"/>
       <c r="I65" s="48" t="n">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="J65" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K65" s="55" t="n"/>
@@ -2882,7 +2886,7 @@
       </c>
       <c r="B66" s="49" t="inlineStr">
         <is>
-          <t>JET CHISEL PNEUMATIC, MODEL JEX-24</t>
+          <t>DRYWALL SCREWS, 25MM, 500PCS</t>
         </is>
       </c>
       <c r="C66" s="50" t="n"/>
@@ -2890,17 +2894,17 @@
       <c r="E66" s="49" t="n"/>
       <c r="F66" s="49" t="inlineStr">
         <is>
-          <t>590463 IMPA MAKER: IMPA CATALOG</t>
+          <t>617183 SCREWS25MM</t>
         </is>
       </c>
       <c r="G66" s="49" t="n"/>
       <c r="H66" s="49" t="n"/>
       <c r="I66" s="48" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="J66" s="48" t="inlineStr">
         <is>
-          <t>SET</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K66" s="55" t="n"/>
@@ -2914,7 +2918,7 @@
       </c>
       <c r="B67" s="49" t="inlineStr">
         <is>
-          <t>WRENCH ADJUSTABLE HEAVY-DUTY, 150MM</t>
+          <t>DRYWALL TAPE, 50MM, 100M</t>
         </is>
       </c>
       <c r="C67" s="50" t="n"/>
@@ -2922,17 +2926,17 @@
       <c r="E67" s="49" t="n"/>
       <c r="F67" s="49" t="inlineStr">
         <is>
-          <t>611332 IMPA MAKER: IMPA CATALOG</t>
+          <t>617184 TAPEDRYWALL</t>
         </is>
       </c>
       <c r="G67" s="49" t="n"/>
       <c r="H67" s="49" t="n"/>
       <c r="I67" s="48" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J67" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K67" s="55" t="n"/>
@@ -2946,7 +2950,7 @@
       </c>
       <c r="B68" s="49" t="inlineStr">
         <is>
-          <t>WRENCH ADJUSTABLE HEAVY-DUTY, 200MM</t>
+          <t>DRYWALL JOINT COMPOUND, 5L BUCKET</t>
         </is>
       </c>
       <c r="C68" s="50" t="n"/>
@@ -2954,17 +2958,17 @@
       <c r="E68" s="49" t="n"/>
       <c r="F68" s="49" t="inlineStr">
         <is>
-          <t>611333 IMPA MAKER: IMPA CATALOG</t>
+          <t>617185 COMPOUND5L</t>
         </is>
       </c>
       <c r="G68" s="49" t="n"/>
       <c r="H68" s="49" t="n"/>
       <c r="I68" s="48" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="J68" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K68" s="55" t="n"/>
@@ -2978,7 +2982,7 @@
       </c>
       <c r="B69" s="49" t="inlineStr">
         <is>
-          <t>WRENCH OPEN &amp; 12-POINT BOX, 6MM</t>
+          <t>TROWEL FOR PLASTERING, STAINLESS STEEL, 180MM</t>
         </is>
       </c>
       <c r="C69" s="50" t="n"/>
@@ -2986,17 +2990,17 @@
       <c r="E69" s="49" t="n"/>
       <c r="F69" s="49" t="inlineStr">
         <is>
-          <t>610761 IMPA MAKER: IMPA CATALOG</t>
+          <t>617186 TROWELPLASTER</t>
         </is>
       </c>
       <c r="G69" s="49" t="n"/>
       <c r="H69" s="49" t="n"/>
       <c r="I69" s="48" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J69" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K69" s="55" t="n"/>
@@ -3010,7 +3014,7 @@
       </c>
       <c r="B70" s="49" t="inlineStr">
         <is>
-          <t>WRENCH OPEN &amp; 12-POINT BOX, 7MM</t>
+          <t>PLASTER MIX, 25KG BAG</t>
         </is>
       </c>
       <c r="C70" s="50" t="n"/>
@@ -3018,17 +3022,17 @@
       <c r="E70" s="49" t="n"/>
       <c r="F70" s="49" t="inlineStr">
         <is>
-          <t>610762 IMPA MAKER: IMPA CATALOG</t>
+          <t>617187 PLASTER25</t>
         </is>
       </c>
       <c r="G70" s="49" t="n"/>
       <c r="H70" s="49" t="n"/>
       <c r="I70" s="48" t="n">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="J70" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>bags</t>
         </is>
       </c>
       <c r="K70" s="55" t="n"/>
@@ -3042,7 +3046,7 @@
       </c>
       <c r="B71" s="49" t="inlineStr">
         <is>
-          <t>WRENCH OPEN &amp; 12-POINT BOX, 8MM</t>
+          <t>STUCCO MATERIALS, 25KG BAG</t>
         </is>
       </c>
       <c r="C71" s="50" t="n"/>
@@ -3050,17 +3054,17 @@
       <c r="E71" s="49" t="n"/>
       <c r="F71" s="49" t="inlineStr">
         <is>
-          <t>610763 IMPA MAKER: IMPA CATALOG</t>
+          <t>617188 STUCCO25</t>
         </is>
       </c>
       <c r="G71" s="49" t="n"/>
       <c r="H71" s="49" t="n"/>
       <c r="I71" s="48" t="n">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="J71" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>bags</t>
         </is>
       </c>
       <c r="K71" s="55" t="n"/>
@@ -3074,7 +3078,7 @@
       </c>
       <c r="B72" s="49" t="inlineStr">
         <is>
-          <t>WRENCH OPEN &amp; 12-POINT BOX, 10MM</t>
+          <t>CLAMPS, C-CLAMPS, 6”</t>
         </is>
       </c>
       <c r="C72" s="50" t="n"/>
@@ -3082,17 +3086,17 @@
       <c r="E72" s="49" t="n"/>
       <c r="F72" s="49" t="inlineStr">
         <is>
-          <t>610765 IMPA MAKER: IMPA CATALOG</t>
+          <t>617189 CCLAMPS6</t>
         </is>
       </c>
       <c r="G72" s="49" t="n"/>
       <c r="H72" s="49" t="n"/>
       <c r="I72" s="48" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="J72" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K72" s="55" t="n"/>
@@ -3106,7 +3110,7 @@
       </c>
       <c r="B73" s="49" t="inlineStr">
         <is>
-          <t>WRENCH OPEN &amp; 12-POINT BOX, 13MM</t>
+          <t>VICE GRIPS, 10”</t>
         </is>
       </c>
       <c r="C73" s="50" t="n"/>
@@ -3114,17 +3118,17 @@
       <c r="E73" s="49" t="n"/>
       <c r="F73" s="49" t="inlineStr">
         <is>
-          <t>610768 IMPA MAKER: IMPA CATALOG</t>
+          <t>617190 VICEGRIPS10</t>
         </is>
       </c>
       <c r="G73" s="49" t="n"/>
       <c r="H73" s="49" t="n"/>
       <c r="I73" s="48" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="J73" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K73" s="55" t="n"/>
@@ -3138,7 +3142,7 @@
       </c>
       <c r="B74" s="49" t="inlineStr">
         <is>
-          <t>CUTTER BOLT ANGLE EDGE 600MM</t>
+          <t>PLIERS, NEEDLE NOSE, 8”</t>
         </is>
       </c>
       <c r="C74" s="50" t="n"/>
@@ -3146,17 +3150,17 @@
       <c r="E74" s="49" t="n"/>
       <c r="F74" s="49" t="inlineStr">
         <is>
-          <t>611892 IMPA MAKER: IMPA CATALOG</t>
+          <t>617132 PLIERS8</t>
         </is>
       </c>
       <c r="G74" s="49" t="n"/>
       <c r="H74" s="49" t="n"/>
       <c r="I74" s="48" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="J74" s="48" t="inlineStr">
         <is>
-          <t>PRS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K74" s="55" t="n"/>
@@ -3170,7 +3174,7 @@
       </c>
       <c r="B75" s="49" t="inlineStr">
         <is>
-          <t>HAMMER CARPENTER 450GRM</t>
+          <t>NAIL GUN, CORDLESS</t>
         </is>
       </c>
       <c r="C75" s="50" t="n"/>
@@ -3178,17 +3182,17 @@
       <c r="E75" s="49" t="n"/>
       <c r="F75" s="49" t="inlineStr">
         <is>
-          <t>612621 IMPA MAKER: IMPA CATALOG</t>
+          <t>617133 NAILGUNCORD</t>
         </is>
       </c>
       <c r="G75" s="49" t="n"/>
       <c r="H75" s="49" t="n"/>
       <c r="I75" s="48" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J75" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K75" s="55" t="n"/>
@@ -3202,7 +3206,7 @@
       </c>
       <c r="B76" s="49" t="inlineStr">
         <is>
-          <t>BAR STRAIGHT PINCH&amp;CHISEL END, 1200MM</t>
+          <t>NAILS, 50MM, 1KG PACK</t>
         </is>
       </c>
       <c r="C76" s="50" t="n"/>
@@ -3210,17 +3214,17 @@
       <c r="E76" s="49" t="n"/>
       <c r="F76" s="49" t="inlineStr">
         <is>
-          <t>612867 IMPA MAKER: IMPA CATALOG</t>
+          <t>617134 NAIL50MM1KG</t>
         </is>
       </c>
       <c r="G76" s="49" t="n"/>
       <c r="H76" s="49" t="n"/>
       <c r="I76" s="48" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="J76" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>packs</t>
         </is>
       </c>
       <c r="K76" s="55" t="n"/>
@@ -3234,7 +3238,7 @@
       </c>
       <c r="B77" s="49" t="inlineStr">
         <is>
-          <t>STENCIL LETTER ADJUSTABLE, BRASS A-Z &amp; 0-9 60MM 76S</t>
+          <t>BOLTS, M10X40MM, GALVANIZED</t>
         </is>
       </c>
       <c r="C77" s="50" t="n"/>
@@ -3242,17 +3246,17 @@
       <c r="E77" s="49" t="n"/>
       <c r="F77" s="49" t="inlineStr">
         <is>
-          <t>613138 IMPA MAKER: IMPA CATALOG</t>
+          <t>617135 BOLTM10X40MM</t>
         </is>
       </c>
       <c r="G77" s="49" t="n"/>
       <c r="H77" s="49" t="n"/>
       <c r="I77" s="48" t="n">
-        <v>2</v>
+        <v>100</v>
       </c>
       <c r="J77" s="48" t="inlineStr">
         <is>
-          <t>SET</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K77" s="55" t="n"/>
@@ -3266,7 +3270,7 @@
       </c>
       <c r="B78" s="49" t="inlineStr">
         <is>
-          <t>STENCIL LETTER ADJUSTABLE, BRASS A-Z &amp; 0-9 100MM 76S</t>
+          <t>NUTS, M10, NYLON INSERT</t>
         </is>
       </c>
       <c r="C78" s="50" t="n"/>
@@ -3274,17 +3278,17 @@
       <c r="E78" s="49" t="n"/>
       <c r="F78" s="49" t="inlineStr">
         <is>
-          <t>613140 IMPA MAKER: IMPA CATALOG</t>
+          <t>617136 NUTM10NYLON</t>
         </is>
       </c>
       <c r="G78" s="49" t="n"/>
       <c r="H78" s="49" t="n"/>
       <c r="I78" s="48" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="J78" s="48" t="inlineStr">
         <is>
-          <t>SET</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K78" s="55" t="n"/>
@@ -3298,7 +3302,7 @@
       </c>
       <c r="B79" s="49" t="inlineStr">
         <is>
-          <t>SHOVEL POLYCARBONATE SQUARE, 1200MM</t>
+          <t>WASHERS, M10, STEEL</t>
         </is>
       </c>
       <c r="C79" s="50" t="n"/>
@@ -3306,17 +3310,17 @@
       <c r="E79" s="49" t="n"/>
       <c r="F79" s="49" t="inlineStr">
         <is>
-          <t>613689 IMPA MAKER: IMPA CATALOG</t>
+          <t>617137 WASHERSTEEL</t>
         </is>
       </c>
       <c r="G79" s="49" t="n"/>
       <c r="H79" s="49" t="n"/>
       <c r="I79" s="48" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="J79" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K79" s="55" t="n"/>
@@ -3330,7 +3334,7 @@
       </c>
       <c r="B80" s="49" t="inlineStr">
         <is>
-          <t>VISE BENCH PARALLEL, SQUARE-CYLINDER 103X117X76MM</t>
+          <t>SCREWDRIVER SET, PHILLIPS &amp; FLATHEAD</t>
         </is>
       </c>
       <c r="C80" s="50" t="n"/>
@@ -3338,17 +3342,17 @@
       <c r="E80" s="49" t="n"/>
       <c r="F80" s="49" t="inlineStr">
         <is>
-          <t>613774 IMPA MAKER: IMPA CATALOG</t>
+          <t>617138 SCREWDRIVERSET</t>
         </is>
       </c>
       <c r="G80" s="49" t="n"/>
       <c r="H80" s="49" t="n"/>
       <c r="I80" s="48" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="J80" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K80" s="55" t="n"/>
@@ -3362,25 +3366,29 @@
       </c>
       <c r="B81" s="49" t="inlineStr">
         <is>
-          <t>SAND PAPER ABRASIVE 230X280MM, GRIT 180</t>
+          <t>IMPACT DRIVER, CORDLESS</t>
         </is>
       </c>
       <c r="C81" s="50" t="n"/>
       <c r="D81" s="51" t="n"/>
-      <c r="E81" s="49" t="n"/>
+      <c r="E81" s="49" t="inlineStr">
+        <is>
+          <t>PS-4000X</t>
+        </is>
+      </c>
       <c r="F81" s="49" t="inlineStr">
         <is>
-          <t>614758 IMPA MAKER: IMPA CATALOG</t>
+          <t>617139 IMPACTDRIVER</t>
         </is>
       </c>
       <c r="G81" s="49" t="n"/>
       <c r="H81" s="49" t="n"/>
       <c r="I81" s="48" t="n">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="J81" s="48" t="inlineStr">
         <is>
-          <t>SHT</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K81" s="55" t="n"/>
@@ -3394,7 +3402,7 @@
       </c>
       <c r="B82" s="49" t="inlineStr">
         <is>
-          <t>SAND PAPER ABRASIVE 230X280MM, GRIT #400</t>
+          <t>ELECTRIC DRILL, 650W</t>
         </is>
       </c>
       <c r="C82" s="50" t="n"/>
@@ -3402,17 +3410,17 @@
       <c r="E82" s="49" t="n"/>
       <c r="F82" s="49" t="inlineStr">
         <is>
-          <t>614762 IMPA MAKER: IMPA CATALOG</t>
+          <t>617140 ELECTRICDRILL650W</t>
         </is>
       </c>
       <c r="G82" s="49" t="n"/>
       <c r="H82" s="49" t="n"/>
       <c r="I82" s="48" t="n">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="J82" s="48" t="inlineStr">
         <is>
-          <t>SHT</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K82" s="55" t="n"/>
@@ -3426,7 +3434,7 @@
       </c>
       <c r="B83" s="49" t="inlineStr">
         <is>
-          <t>WHEEL FREE SWIVEL TYPE 130MM, FOR PLATFORM TRUCK</t>
+          <t>DRILL BITS, WOOD, 6MM-12MM</t>
         </is>
       </c>
       <c r="C83" s="50" t="n"/>
@@ -3434,17 +3442,17 @@
       <c r="E83" s="49" t="n"/>
       <c r="F83" s="49" t="inlineStr">
         <is>
-          <t>617167 IMPA MAKER: IMPA CATALOG</t>
+          <t>617141 DRILLBITS6MM12MM</t>
         </is>
       </c>
       <c r="G83" s="49" t="n"/>
       <c r="H83" s="49" t="n"/>
       <c r="I83" s="48" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="J83" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K83" s="55" t="n"/>
@@ -3458,7 +3466,7 @@
       </c>
       <c r="B84" s="49" t="inlineStr">
         <is>
-          <t>GREASE GUN W/FLEX. PIPE&amp;SWIVEL, JOINT FOR AIR GREASE PUMP</t>
+          <t>LADDER LEVELING FEET, SET OF 4</t>
         </is>
       </c>
       <c r="C84" s="50" t="n"/>
@@ -3466,17 +3474,17 @@
       <c r="E84" s="49" t="n"/>
       <c r="F84" s="49" t="inlineStr">
         <is>
-          <t>617412 IMPA MAKER: IMPA CATALOG</t>
+          <t>617142 LADDERFEET4</t>
         </is>
       </c>
       <c r="G84" s="49" t="n"/>
       <c r="H84" s="49" t="n"/>
       <c r="I84" s="48" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J84" s="48" t="inlineStr">
         <is>
-          <t>SET</t>
+          <t>sets</t>
         </is>
       </c>
       <c r="K84" s="55" t="n"/>
@@ -3490,7 +3498,7 @@
       </c>
       <c r="B85" s="49" t="inlineStr">
         <is>
-          <t>QUICK BONDING ADHESIVE, NO.201 20GRM</t>
+          <t>SCAFFOLD PLANKS, WOODEN, 2.4M</t>
         </is>
       </c>
       <c r="C85" s="50" t="n"/>
@@ -3498,17 +3506,17 @@
       <c r="E85" s="49" t="n"/>
       <c r="F85" s="49" t="inlineStr">
         <is>
-          <t>812726 IMPA MAKER: IMPA CATALOG</t>
+          <t>617143 SCAFFOLDPLANKS24M</t>
         </is>
       </c>
       <c r="G85" s="49" t="n"/>
       <c r="H85" s="49" t="n"/>
       <c r="I85" s="48" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="J85" s="48" t="inlineStr">
         <is>
-          <t>TUB</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K85" s="55" t="n"/>
@@ -3522,7 +3530,7 @@
       </c>
       <c r="B86" s="49" t="inlineStr">
         <is>
-          <t>HAMMER BLACKSMITH DOUBLE FACE, WITH HANDLE NO.12 (5.4KGS)</t>
+          <t>SCAFFOLD BRACKETS, STEEL, 600MM</t>
         </is>
       </c>
       <c r="C86" s="50" t="n"/>
@@ -3530,17 +3538,17 @@
       <c r="E86" s="49" t="n"/>
       <c r="F86" s="49" t="inlineStr">
         <is>
-          <t>612528 IMPA MAKER: IMPA CATALOG</t>
+          <t>617144 SCAFFOLDBRACKETS600</t>
         </is>
       </c>
       <c r="G86" s="49" t="n"/>
       <c r="H86" s="49" t="n"/>
       <c r="I86" s="48" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="J86" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K86" s="55" t="n"/>
@@ -3554,7 +3562,7 @@
       </c>
       <c r="B87" s="49" t="inlineStr">
         <is>
-          <t>SHACKLE STRAIGHT HEX HEAD BOLT, S.STEEL SB 12MM SWL 1.0TON</t>
+          <t>SCAFFOLD COUPLERS, CLAMP STYLE</t>
         </is>
       </c>
       <c r="C87" s="50" t="n"/>
@@ -3562,17 +3570,17 @@
       <c r="E87" s="49" t="n"/>
       <c r="F87" s="49" t="inlineStr">
         <is>
-          <t>233521 IMPA MAKER: IMPA CATALOG</t>
+          <t>617145 SCAFFOLDCOUPLER</t>
         </is>
       </c>
       <c r="G87" s="49" t="n"/>
       <c r="H87" s="49" t="n"/>
       <c r="I87" s="48" t="n">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="J87" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K87" s="55" t="n"/>
@@ -3586,7 +3594,7 @@
       </c>
       <c r="B88" s="49" t="inlineStr">
         <is>
-          <t>SHACKLE STRAIGHT HEX HEAD BOLT, S.STEEL SB 18MM SWL 2.0TON</t>
+          <t>ADJUSTABLE SCAFFOLDING JACKS, 1M HEIGHT</t>
         </is>
       </c>
       <c r="C88" s="50" t="n"/>
@@ -3594,17 +3602,17 @@
       <c r="E88" s="49" t="n"/>
       <c r="F88" s="49" t="inlineStr">
         <is>
-          <t>233524 IMPA MAKER: IMPA CATALOG</t>
+          <t>617146 SCAFFOLDJACK1M</t>
         </is>
       </c>
       <c r="G88" s="49" t="n"/>
       <c r="H88" s="49" t="n"/>
       <c r="I88" s="48" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="J88" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K88" s="55" t="n"/>
@@ -3618,7 +3626,7 @@
       </c>
       <c r="B89" s="49" t="inlineStr">
         <is>
-          <t>SHACKLE STRAIGHT HEX HEAD BOLT, S.STEEL SB 34MM SWL 7.0TON</t>
+          <t>HOISTING EQUIPMENT, MANUAL</t>
         </is>
       </c>
       <c r="C89" s="50" t="n"/>
@@ -3626,17 +3634,17 @@
       <c r="E89" s="49" t="n"/>
       <c r="F89" s="49" t="inlineStr">
         <is>
-          <t>233532 IMPA MAKER: IMPA CATALOG</t>
+          <t>617147 HOISTINGEQUIPMENT</t>
         </is>
       </c>
       <c r="G89" s="49" t="n"/>
       <c r="H89" s="49" t="n"/>
       <c r="I89" s="48" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J89" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K89" s="55" t="n"/>
@@ -3650,7 +3658,7 @@
       </c>
       <c r="B90" s="49" t="inlineStr">
         <is>
-          <t>CARGO HOOK SWIVEL EYE WITH, LATCH SWL 2TON</t>
+          <t>CRANE HOOK, 5 TON</t>
         </is>
       </c>
       <c r="C90" s="50" t="n"/>
@@ -3658,7 +3666,7 @@
       <c r="E90" s="49" t="n"/>
       <c r="F90" s="49" t="inlineStr">
         <is>
-          <t>231253 IMPA MAKER: IMPA CATALOG</t>
+          <t>617148 CRANEHOOK5TON</t>
         </is>
       </c>
       <c r="G90" s="49" t="n"/>
@@ -3668,7 +3676,7 @@
       </c>
       <c r="J90" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K90" s="55" t="n"/>
@@ -3682,7 +3690,7 @@
       </c>
       <c r="B91" s="49" t="inlineStr">
         <is>
-          <t>CARGO HOOK SWIVEL EYE WITH, LATCH SWL 1TON</t>
+          <t>WINCH, MANUAL, 1 TON</t>
         </is>
       </c>
       <c r="C91" s="50" t="n"/>
@@ -3690,17 +3698,17 @@
       <c r="E91" s="49" t="n"/>
       <c r="F91" s="49" t="inlineStr">
         <is>
-          <t>231251 IMPA MAKER: IMPA CATALOG</t>
+          <t>617149 WINCHMANUAL1TON</t>
         </is>
       </c>
       <c r="G91" s="49" t="n"/>
       <c r="H91" s="49" t="n"/>
       <c r="I91" s="48" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J91" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K91" s="55" t="n"/>
@@ -3714,7 +3722,7 @@
       </c>
       <c r="B92" s="49" t="inlineStr">
         <is>
-          <t>CARGO HOOK SWIVEL EYE WITH, LATCH LOCK WLL 8.0TON</t>
+          <t>PULLEY SYSTEM, 4-TON CAPACITY</t>
         </is>
       </c>
       <c r="C92" s="50" t="n"/>
@@ -3722,7 +3730,7 @@
       <c r="E92" s="49" t="n"/>
       <c r="F92" s="49" t="inlineStr">
         <is>
-          <t>231265 IMPA MAKER: IMPA CATALOG</t>
+          <t>617150 PULLEYSYSTEM4TON</t>
         </is>
       </c>
       <c r="G92" s="49" t="n"/>
@@ -3732,7 +3740,7 @@
       </c>
       <c r="J92" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K92" s="55" t="n"/>
@@ -3746,7 +3754,7 @@
       </c>
       <c r="B93" s="49" t="inlineStr">
         <is>
-          <t>WASTE BASKET PEDAL FLIP, ST/STEEL 20LTR</t>
+          <t>STEEL CABLE, 8MM DIAMETER, 100M</t>
         </is>
       </c>
       <c r="C93" s="50" t="n"/>
@@ -3754,17 +3762,17 @@
       <c r="E93" s="49" t="n"/>
       <c r="F93" s="49" t="inlineStr">
         <is>
-          <t>174154 IMPA MAKER: IMPA CATALOG</t>
+          <t>617151 STEELCABLE8MM100M</t>
         </is>
       </c>
       <c r="G93" s="49" t="n"/>
       <c r="H93" s="49" t="n"/>
       <c r="I93" s="48" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="J93" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K93" s="55" t="n"/>
@@ -3778,7 +3786,7 @@
       </c>
       <c r="B94" s="49" t="inlineStr">
         <is>
-          <t>WIRE COPPER 0.8MM</t>
+          <t>RATCHET STRAPS, 5M LENGTH</t>
         </is>
       </c>
       <c r="C94" s="50" t="n"/>
@@ -3786,17 +3794,17 @@
       <c r="E94" s="49" t="n"/>
       <c r="F94" s="49" t="inlineStr">
         <is>
-          <t>671856 IMPA MAKER: IMPA CATALOG</t>
+          <t>617152 RATCHETSTRAPS5M</t>
         </is>
       </c>
       <c r="G94" s="49" t="n"/>
       <c r="H94" s="49" t="n"/>
       <c r="I94" s="48" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="J94" s="48" t="inlineStr">
         <is>
-          <t>KGS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K94" s="55" t="n"/>
@@ -3810,25 +3818,29 @@
       </c>
       <c r="B95" s="49" t="inlineStr">
         <is>
-          <t>WIRE COPPER 1.0MM</t>
+          <t>CHAIN SLINGS, 10MM, 2M LENGTH</t>
         </is>
       </c>
       <c r="C95" s="50" t="n"/>
       <c r="D95" s="51" t="n"/>
-      <c r="E95" s="49" t="n"/>
+      <c r="E95" s="49" t="inlineStr">
+        <is>
+          <t>RS-5M-SS</t>
+        </is>
+      </c>
       <c r="F95" s="49" t="inlineStr">
         <is>
-          <t>671858 IMPA MAKER: IMPA CATALOG</t>
+          <t>617153 CHAINSLINGS10MM2M</t>
         </is>
       </c>
       <c r="G95" s="49" t="n"/>
       <c r="H95" s="49" t="n"/>
       <c r="I95" s="48" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J95" s="48" t="inlineStr">
         <is>
-          <t>KGS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K95" s="55" t="n"/>
@@ -3842,25 +3854,29 @@
       </c>
       <c r="B96" s="49" t="inlineStr">
         <is>
-          <t>WIRE COPPER 1.4MM</t>
+          <t>SLINGS, WIRE ROPE, 4MM DIAMETER, 3M LENGTH</t>
         </is>
       </c>
       <c r="C96" s="50" t="n"/>
       <c r="D96" s="51" t="n"/>
-      <c r="E96" s="49" t="n"/>
+      <c r="E96" s="49" t="inlineStr">
+        <is>
+          <t>WR-4-3M</t>
+        </is>
+      </c>
       <c r="F96" s="49" t="inlineStr">
         <is>
-          <t>671860 IMPA MAKER: IMPA CATALOG</t>
+          <t>617154 SLINGWIREROPE4MM3M</t>
         </is>
       </c>
       <c r="G96" s="49" t="n"/>
       <c r="H96" s="49" t="n"/>
       <c r="I96" s="48" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="J96" s="48" t="inlineStr">
         <is>
-          <t>KGS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K96" s="55" t="n"/>
@@ -3874,7 +3890,7 @@
       </c>
       <c r="B97" s="49" t="inlineStr">
         <is>
-          <t>CHISEL SCALER AIR TRELAWNY, IN-LINE VL223 LOW VIB. 2400BPM</t>
+          <t>LOAD TESTING EQUIPMENT, 10 TON CAPACITY</t>
         </is>
       </c>
       <c r="C97" s="50" t="n"/>
@@ -3882,7 +3898,7 @@
       <c r="E97" s="49" t="n"/>
       <c r="F97" s="49" t="inlineStr">
         <is>
-          <t>590519 IMPA MAKER: IMPA CATALOG</t>
+          <t>617155 LOADTESTING10TON</t>
         </is>
       </c>
       <c r="G97" s="49" t="n"/>
@@ -3892,7 +3908,7 @@
       </c>
       <c r="J97" s="48" t="inlineStr">
         <is>
-          <t>SET</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K97" s="55" t="n"/>
@@ -3906,7 +3922,7 @@
       </c>
       <c r="B98" s="49" t="inlineStr">
         <is>
-          <t>TAPE OIL GAUGE ST/STEEL, METRIC 20M</t>
+          <t>SAFETY HARNESS, FULL BODY, SIZE M/L</t>
         </is>
       </c>
       <c r="C98" s="50" t="n"/>
@@ -3914,17 +3930,17 @@
       <c r="E98" s="49" t="n"/>
       <c r="F98" s="49" t="inlineStr">
         <is>
-          <t>650872 IMPA MAKER: IMPA CATALOG</t>
+          <t>617156 SAFETYHARNESSM/L</t>
         </is>
       </c>
       <c r="G98" s="49" t="n"/>
       <c r="H98" s="49" t="n"/>
       <c r="I98" s="48" t="n">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="J98" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K98" s="55" t="n"/>
@@ -3938,7 +3954,7 @@
       </c>
       <c r="B99" s="49" t="inlineStr">
         <is>
-          <t>TAPE OIL GAUGE ST/STEEL, METRIC 30M</t>
+          <t>FALL PROTECTION EQUIPMENT, ROOF EDGE</t>
         </is>
       </c>
       <c r="C99" s="50" t="n"/>
@@ -3946,17 +3962,17 @@
       <c r="E99" s="49" t="n"/>
       <c r="F99" s="49" t="inlineStr">
         <is>
-          <t>650873 IMPA MAKER: IMPA CATALOG</t>
+          <t>617157 FALLPROTECTIONROOF</t>
         </is>
       </c>
       <c r="G99" s="49" t="n"/>
       <c r="H99" s="49" t="n"/>
       <c r="I99" s="48" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="J99" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K99" s="55" t="n"/>
@@ -3970,7 +3986,7 @@
       </c>
       <c r="B100" s="49" t="inlineStr">
         <is>
-          <t>WATER FINDING PASTE 75GRM, YELLOW TO RED</t>
+          <t>REFLECTIVE SAFETY TAPE, 50MM X 50M</t>
         </is>
       </c>
       <c r="C100" s="50" t="n"/>
@@ -3978,17 +3994,17 @@
       <c r="E100" s="49" t="n"/>
       <c r="F100" s="49" t="inlineStr">
         <is>
-          <t>650890 IMPA MAKER: IMPA CATALOG</t>
+          <t>617158 SAFETAPE50MM50M</t>
         </is>
       </c>
       <c r="G100" s="49" t="n"/>
       <c r="H100" s="49" t="n"/>
       <c r="I100" s="48" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J100" s="48" t="inlineStr">
         <is>
-          <t>TUB</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K100" s="55" t="n"/>
@@ -4002,7 +4018,7 @@
       </c>
       <c r="B101" s="49" t="inlineStr">
         <is>
-          <t>GASOLINE &amp; OIL FINDING PASTE, 75GRM BLUE TO RED</t>
+          <t>CONCRETE CURING BLANKETS, 3M X 3M</t>
         </is>
       </c>
       <c r="C101" s="50" t="n"/>
@@ -4010,17 +4026,17 @@
       <c r="E101" s="49" t="n"/>
       <c r="F101" s="49" t="inlineStr">
         <is>
-          <t>650891 IMPA MAKER: IMPA CATALOG</t>
+          <t>617159 CURINGBLANKET3MX3M</t>
         </is>
       </c>
       <c r="G101" s="49" t="n"/>
       <c r="H101" s="49" t="n"/>
       <c r="I101" s="48" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="J101" s="48" t="inlineStr">
         <is>
-          <t>TUB</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K101" s="55" t="n"/>
@@ -4034,7 +4050,7 @@
       </c>
       <c r="B102" s="49" t="inlineStr">
         <is>
-          <t>TRY SQUARE PRECISION WITH BASE, 1ST-GRADE(+_0.02) 200X130MM</t>
+          <t>CONCRETE SAW, 350MM BLADE</t>
         </is>
       </c>
       <c r="C102" s="50" t="n"/>
@@ -4042,7 +4058,7 @@
       <c r="E102" s="49" t="n"/>
       <c r="F102" s="49" t="inlineStr">
         <is>
-          <t>650971 IMPA MAKER: IMPA CATALOG</t>
+          <t>617160 CONCRETESAW350MM</t>
         </is>
       </c>
       <c r="G102" s="49" t="n"/>
@@ -4052,7 +4068,7 @@
       </c>
       <c r="J102" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K102" s="55" t="n"/>
@@ -4066,7 +4082,7 @@
       </c>
       <c r="B103" s="49" t="inlineStr">
         <is>
-          <t>TRY SQUARE PRECISION WITH BASE, 1ST-GRADE(+_0.025) 300X200MM</t>
+          <t>REBAR CUTTER, MANUAL, 16MM CAPACITY</t>
         </is>
       </c>
       <c r="C103" s="50" t="n"/>
@@ -4074,7 +4090,7 @@
       <c r="E103" s="49" t="n"/>
       <c r="F103" s="49" t="inlineStr">
         <is>
-          <t>650973 IMPA MAKER: IMPA CATALOG</t>
+          <t>617161 REBARCUTTER16MM</t>
         </is>
       </c>
       <c r="G103" s="49" t="n"/>
@@ -4084,7 +4100,7 @@
       </c>
       <c r="J103" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K103" s="55" t="n"/>
@@ -4098,7 +4114,7 @@
       </c>
       <c r="B104" s="49" t="inlineStr">
         <is>
-          <t>HARNESS S'GL D-RING WORKMAN,MSA PREMIER QWIK-FIT L 10115543</t>
+          <t>REBAR BENDER, 12MM CAPACITY</t>
         </is>
       </c>
       <c r="C104" s="50" t="n"/>
@@ -4106,17 +4122,17 @@
       <c r="E104" s="49" t="n"/>
       <c r="F104" s="49" t="inlineStr">
         <is>
-          <t>311516 IMPA MAKER: IMPA CATALOG</t>
+          <t>617162 REBARBENDER12MM</t>
         </is>
       </c>
       <c r="G104" s="49" t="n"/>
       <c r="H104" s="49" t="n"/>
       <c r="I104" s="48" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J104" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K104" s="55" t="n"/>
@@ -4130,7 +4146,7 @@
       </c>
       <c r="B105" s="49" t="inlineStr">
         <is>
-          <t>HARNESS S'GL D-RING WORKMAN,MSA PREMIER QWIK-FIT M 10115542</t>
+          <t>FLOOR TILES, CERAMIC, 300X300MM</t>
         </is>
       </c>
       <c r="C105" s="50" t="n"/>
@@ -4138,17 +4154,17 @@
       <c r="E105" s="49" t="n"/>
       <c r="F105" s="49" t="inlineStr">
         <is>
-          <t>311515 IMPA MAKER: IMPA CATALOG</t>
+          <t>617163 FLOORTILECERAMIC</t>
         </is>
       </c>
       <c r="G105" s="49" t="n"/>
       <c r="H105" s="49" t="n"/>
       <c r="I105" s="48" t="n">
-        <v>3</v>
+        <v>500</v>
       </c>
       <c r="J105" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K105" s="55" t="n"/>
@@ -4162,7 +4178,7 @@
       </c>
       <c r="B106" s="49" t="inlineStr">
         <is>
-          <t>GOGGLE ULTRASONIC UVEX 9302, ORANGE FRAME</t>
+          <t>TILE ADHESIVE, 25KG BAG</t>
         </is>
       </c>
       <c r="C106" s="50" t="n"/>
@@ -4170,17 +4186,17 @@
       <c r="E106" s="49" t="n"/>
       <c r="F106" s="49" t="inlineStr">
         <is>
-          <t>311101 IMPA MAKER: IMPA CATALOG</t>
+          <t>617164 TILEADHESIVE25KG</t>
         </is>
       </c>
       <c r="G106" s="49" t="n"/>
       <c r="H106" s="49" t="n"/>
       <c r="I106" s="48" t="n">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="J106" s="48" t="inlineStr">
         <is>
-          <t>PRS</t>
+          <t>bags</t>
         </is>
       </c>
       <c r="K106" s="55" t="n"/>
@@ -4194,7 +4210,7 @@
       </c>
       <c r="B107" s="49" t="inlineStr">
         <is>
-          <t>SHACKLE FAIRLEAD MANDAL 120M, WITH DNV CERTIFICATE</t>
+          <t>TILE GROUT, 5KG BUCKET</t>
         </is>
       </c>
       <c r="C107" s="50" t="n"/>
@@ -4202,17 +4218,17 @@
       <c r="E107" s="49" t="n"/>
       <c r="F107" s="49" t="inlineStr">
         <is>
-          <t>211157 IMPA MAKER: IMPA CATALOG</t>
+          <t>617165 TILEGROUT5KG</t>
         </is>
       </c>
       <c r="G107" s="49" t="n"/>
       <c r="H107" s="49" t="n"/>
       <c r="I107" s="48" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="J107" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>buckets</t>
         </is>
       </c>
       <c r="K107" s="55" t="n"/>
@@ -4226,7 +4242,7 @@
       </c>
       <c r="B108" s="49" t="inlineStr">
         <is>
-          <t>IMPACT WRENCH PNEUMATIC 13MM, 12.7MM2 DRIVE</t>
+          <t>TILE CUTTER, MANUAL, 600MM</t>
         </is>
       </c>
       <c r="C108" s="50" t="n"/>
@@ -4234,17 +4250,17 @@
       <c r="E108" s="49" t="n"/>
       <c r="F108" s="49" t="inlineStr">
         <is>
-          <t>590101 IMPA MAKER: IMPA CATALOG</t>
+          <t>617166 TILECUTTER600MM</t>
         </is>
       </c>
       <c r="G108" s="49" t="n"/>
       <c r="H108" s="49" t="n"/>
       <c r="I108" s="48" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J108" s="48" t="inlineStr">
         <is>
-          <t>SET</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K108" s="55" t="n"/>
@@ -4258,7 +4274,7 @@
       </c>
       <c r="B109" s="49" t="inlineStr">
         <is>
-          <t>SOCKET FOR IMPACT WRENCH, 12.7MM2 DR. X 17MM</t>
+          <t>CEMENT MIXER PARTS, MOTOR, 230V</t>
         </is>
       </c>
       <c r="C109" s="50" t="n"/>
@@ -4266,17 +4282,17 @@
       <c r="E109" s="49" t="n"/>
       <c r="F109" s="49" t="inlineStr">
         <is>
-          <t>590218 IMPA MAKER: IMPA CATALOG</t>
+          <t>617167 CEMENTMOTORS230V</t>
         </is>
       </c>
       <c r="G109" s="49" t="n"/>
       <c r="H109" s="49" t="n"/>
       <c r="I109" s="48" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J109" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K109" s="55" t="n"/>
@@ -4290,7 +4306,7 @@
       </c>
       <c r="B110" s="49" t="inlineStr">
         <is>
-          <t>SOCKET FOR IMPACT WRENCH, 12.7MM2 DR. X 19MM</t>
+          <t>ANGLE IRON, GALVANIZED, 50MM X 50MM</t>
         </is>
       </c>
       <c r="C110" s="50" t="n"/>
@@ -4298,17 +4314,17 @@
       <c r="E110" s="49" t="n"/>
       <c r="F110" s="49" t="inlineStr">
         <is>
-          <t>590219 IMPA MAKER: IMPA CATALOG</t>
+          <t>617168 ANGLEIRON50MM50MM</t>
         </is>
       </c>
       <c r="G110" s="49" t="n"/>
       <c r="H110" s="49" t="n"/>
       <c r="I110" s="48" t="n">
-        <v>2</v>
+        <v>50</v>
       </c>
       <c r="J110" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K110" s="55" t="n"/>
@@ -4322,7 +4338,7 @@
       </c>
       <c r="B111" s="49" t="inlineStr">
         <is>
-          <t>SOCKET FOR IMPACT WRENCH, 12.7MM2 DR. X 21MM</t>
+          <t>CHANNEL STEEL, 100MM X 50MM</t>
         </is>
       </c>
       <c r="C111" s="50" t="n"/>
@@ -4330,17 +4346,17 @@
       <c r="E111" s="49" t="n"/>
       <c r="F111" s="49" t="inlineStr">
         <is>
-          <t>590220 IMPA MAKER: IMPA CATALOG</t>
+          <t>617169 CHANNELSTEEL100MM</t>
         </is>
       </c>
       <c r="G111" s="49" t="n"/>
       <c r="H111" s="49" t="n"/>
       <c r="I111" s="48" t="n">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="J111" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K111" s="55" t="n"/>
@@ -4354,7 +4370,7 @@
       </c>
       <c r="B112" s="49" t="inlineStr">
         <is>
-          <t>SOCKET FOR IMPACT WRENCH, 12.7MM2 DR. X 23MM</t>
+          <t>STEEL PLATES, 10MM THICK, 1000X2000MM</t>
         </is>
       </c>
       <c r="C112" s="50" t="n"/>
@@ -4362,17 +4378,17 @@
       <c r="E112" s="49" t="n"/>
       <c r="F112" s="49" t="inlineStr">
         <is>
-          <t>590222 IMPA MAKER: IMPA CATALOG</t>
+          <t>617170 STEELPLATES10MM1000X2000</t>
         </is>
       </c>
       <c r="G112" s="49" t="n"/>
       <c r="H112" s="49" t="n"/>
       <c r="I112" s="48" t="n">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="J112" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K112" s="55" t="n"/>
@@ -4386,7 +4402,7 @@
       </c>
       <c r="B113" s="49" t="inlineStr">
         <is>
-          <t>SOCKET FOR IMPACT WRENCH, 12.7MM2 DR. X 24MM</t>
+          <t>STEEL RODS, 12MM DIAMETER, 6M LENGTH</t>
         </is>
       </c>
       <c r="C113" s="50" t="n"/>
@@ -4394,17 +4410,17 @@
       <c r="E113" s="49" t="n"/>
       <c r="F113" s="49" t="inlineStr">
         <is>
-          <t>590223 IMPA MAKER: IMPA CATALOG</t>
+          <t>617171 STEELRODS12MM6M</t>
         </is>
       </c>
       <c r="G113" s="49" t="n"/>
       <c r="H113" s="49" t="n"/>
       <c r="I113" s="48" t="n">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="J113" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K113" s="55" t="n"/>
@@ -4418,25 +4434,29 @@
       </c>
       <c r="B114" s="49" t="inlineStr">
         <is>
-          <t>SOCKET FOR IMPACT WRENCH, 12.7MM2 DR. X 26MM</t>
+          <t>WELDING GLOVES, LEATHER, SIZE L</t>
         </is>
       </c>
       <c r="C114" s="50" t="n"/>
       <c r="D114" s="51" t="n"/>
-      <c r="E114" s="49" t="n"/>
+      <c r="E114" s="49" t="inlineStr">
+        <is>
+          <t>CS-10-2M</t>
+        </is>
+      </c>
       <c r="F114" s="49" t="inlineStr">
         <is>
-          <t>590224 IMPA MAKER: IMPA CATALOG</t>
+          <t>617172 WELDINGGLOVESL</t>
         </is>
       </c>
       <c r="G114" s="49" t="n"/>
       <c r="H114" s="49" t="n"/>
       <c r="I114" s="48" t="n">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="J114" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K114" s="55" t="n"/>
@@ -4450,7 +4470,7 @@
       </c>
       <c r="B115" s="49" t="inlineStr">
         <is>
-          <t>SOCKET FOR IMPACT WRENCH, 12.7MM2 DR. X 29MM</t>
+          <t>ARC WELDING RODS, 2.5MM, 5KG BOX</t>
         </is>
       </c>
       <c r="C115" s="50" t="n"/>
@@ -4458,17 +4478,17 @@
       <c r="E115" s="49" t="n"/>
       <c r="F115" s="49" t="inlineStr">
         <is>
-          <t>590226 IMPA MAKER: IMPA CATALOG</t>
+          <t>617173 ARCWELDINGRODS</t>
         </is>
       </c>
       <c r="G115" s="49" t="n"/>
       <c r="H115" s="49" t="n"/>
       <c r="I115" s="48" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="J115" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>boxes</t>
         </is>
       </c>
       <c r="K115" s="55" t="n"/>
@@ -4482,7 +4502,7 @@
       </c>
       <c r="B116" s="49" t="inlineStr">
         <is>
-          <t>SOCKET FOR IMPACT WRENCH, 12.7MM2 DR. X 30MM</t>
+          <t>MIG WELDING WIRE, 0.8MM, 1KG ROLL</t>
         </is>
       </c>
       <c r="C116" s="50" t="n"/>
@@ -4490,17 +4510,17 @@
       <c r="E116" s="49" t="n"/>
       <c r="F116" s="49" t="inlineStr">
         <is>
-          <t>590227 IMPA MAKER: IMPA CATALOG</t>
+          <t>617174 MIGWELDINGWIRE</t>
         </is>
       </c>
       <c r="G116" s="49" t="n"/>
       <c r="H116" s="49" t="n"/>
       <c r="I116" s="48" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="J116" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>rolls</t>
         </is>
       </c>
       <c r="K116" s="55" t="n"/>
@@ -4514,7 +4534,7 @@
       </c>
       <c r="B117" s="49" t="inlineStr">
         <is>
-          <t>SOCKET FOR IMPACT WRENCH, 12.7MM2 DR. X 32MM</t>
+          <t>TIG WELDING TORCH, AIR-COOLED</t>
         </is>
       </c>
       <c r="C117" s="50" t="n"/>
@@ -4522,17 +4542,17 @@
       <c r="E117" s="49" t="n"/>
       <c r="F117" s="49" t="inlineStr">
         <is>
-          <t>590228 IMPA MAKER: IMPA CATALOG</t>
+          <t>617175 TIGWELDINGTORCH</t>
         </is>
       </c>
       <c r="G117" s="49" t="n"/>
       <c r="H117" s="49" t="n"/>
       <c r="I117" s="48" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J117" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K117" s="55" t="n"/>
@@ -4546,7 +4566,7 @@
       </c>
       <c r="B118" s="49" t="inlineStr">
         <is>
-          <t>SOAP HAND IN PUMP DISPENSER, JELL 250ML</t>
+          <t>WELDING HELMET, AUTO-DARKENING</t>
         </is>
       </c>
       <c r="C118" s="50" t="n"/>
@@ -4554,17 +4574,17 @@
       <c r="E118" s="49" t="n"/>
       <c r="F118" s="49" t="inlineStr">
         <is>
-          <t>550291 IMPA MAKER: IMPA CATALOG</t>
+          <t>617176 WELDINGHELMETAUTO</t>
         </is>
       </c>
       <c r="G118" s="49" t="n"/>
       <c r="H118" s="49" t="n"/>
       <c r="I118" s="48" t="n">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="J118" s="48" t="inlineStr">
         <is>
-          <t>BTL</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K118" s="55" t="n"/>
@@ -4578,7 +4598,7 @@
       </c>
       <c r="B119" s="49" t="inlineStr">
         <is>
-          <t>LINE COUPLER BRANCH PIPING, 200L 4X20SM / 1X40SM &amp; 1X400PM</t>
+          <t>SAFETY GOGGLES, UV PROTECTED</t>
         </is>
       </c>
       <c r="C119" s="50" t="n"/>
@@ -4586,17 +4606,17 @@
       <c r="E119" s="49" t="n"/>
       <c r="F119" s="49" t="inlineStr">
         <is>
-          <t>351653 IMPA MAKER: IMPA CATALOG</t>
+          <t>617177 SAFETYGOGGLESUV</t>
         </is>
       </c>
       <c r="G119" s="49" t="n"/>
       <c r="H119" s="49" t="n"/>
       <c r="I119" s="48" t="n">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="J119" s="48" t="inlineStr">
         <is>
-          <t>SET</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K119" s="55" t="n"/>
@@ -4610,7 +4630,7 @@
       </c>
       <c r="B120" s="49" t="inlineStr">
         <is>
-          <t>PACKING DOOR WATERTIGHT, EPDM RUBBER 40X20MM L:10M</t>
+          <t>DUST MASKS, FFP2, 10-PACK</t>
         </is>
       </c>
       <c r="C120" s="50" t="n"/>
@@ -4618,17 +4638,17 @@
       <c r="E120" s="49" t="n"/>
       <c r="F120" s="49" t="inlineStr">
         <is>
-          <t>815009 IMPA MAKER: IMPA CATALOG</t>
+          <t>617178 DUSTMASKFFP2</t>
         </is>
       </c>
       <c r="G120" s="49" t="n"/>
       <c r="H120" s="49" t="n"/>
       <c r="I120" s="48" t="n">
-        <v>80</v>
+        <v>5</v>
       </c>
       <c r="J120" s="48" t="inlineStr">
         <is>
-          <t>LGH</t>
+          <t>packs</t>
         </is>
       </c>
       <c r="K120" s="55" t="n"/>
@@ -4642,7 +4662,7 @@
       </c>
       <c r="B121" s="49" t="inlineStr">
         <is>
-          <t>PACKING DOOR WATERTIGHT, EPDM RUBBER 40X40MM L:10M</t>
+          <t>RESPIRATORS FOR WELDING, NIOSH APPROVED</t>
         </is>
       </c>
       <c r="C121" s="50" t="n"/>
@@ -4650,17 +4670,17 @@
       <c r="E121" s="49" t="n"/>
       <c r="F121" s="49" t="inlineStr">
         <is>
-          <t>815013 IMPA MAKER: IMPA CATALOG</t>
+          <t>617179 RESPIRATORSWELDING</t>
         </is>
       </c>
       <c r="G121" s="49" t="n"/>
       <c r="H121" s="49" t="n"/>
       <c r="I121" s="48" t="n">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="J121" s="48" t="inlineStr">
         <is>
-          <t>LGH</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K121" s="55" t="n"/>
@@ -4674,7 +4694,7 @@
       </c>
       <c r="B122" s="49" t="inlineStr">
         <is>
-          <t>SCREW TAPPING WITH FURTHER, DETAIL</t>
+          <t>HEAT GUN, 1500W</t>
         </is>
       </c>
       <c r="C122" s="50" t="n"/>
@@ -4682,17 +4702,17 @@
       <c r="E122" s="49" t="n"/>
       <c r="F122" s="49" t="inlineStr">
         <is>
-          <t>694401 IMPA MAKER: IMPA CATALOG</t>
+          <t>617180 HEATGUN1500W</t>
         </is>
       </c>
       <c r="G122" s="49" t="n"/>
       <c r="H122" s="49" t="n"/>
       <c r="I122" s="48" t="n">
-        <v>300</v>
+        <v>5</v>
       </c>
       <c r="J122" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K122" s="55" t="n"/>
@@ -4706,7 +4726,7 @@
       </c>
       <c r="B123" s="49" t="inlineStr">
         <is>
-          <t>DOUBLE SLING FOR SAFETY HARNESS TECHNOALP LN202</t>
+          <t>PVC WELDING EQUIPMENT, ELECTRIC, 1600W</t>
         </is>
       </c>
       <c r="C123" s="50" t="n"/>
@@ -4714,17 +4734,17 @@
       <c r="E123" s="49" t="n"/>
       <c r="F123" s="49" t="inlineStr">
         <is>
-          <t>SKU:15.044 MAKER: PV FIRMA TECHNICAL STORE</t>
+          <t>617181 PVCWELDING1600W</t>
         </is>
       </c>
       <c r="G123" s="49" t="n"/>
       <c r="H123" s="49" t="n"/>
       <c r="I123" s="48" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="J123" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K123" s="55" t="n"/>
@@ -4738,7 +4758,7 @@
       </c>
       <c r="B124" s="49" t="inlineStr">
         <is>
-          <t>SLING BELT POLYESTER, WIDTH 50MM X L 6M</t>
+          <t>CONSTRUCTION SANDBAGS, 50KG</t>
         </is>
       </c>
       <c r="C124" s="50" t="n"/>
@@ -4746,17 +4766,17 @@
       <c r="E124" s="49" t="n"/>
       <c r="F124" s="49" t="inlineStr">
         <is>
-          <t>232148 IMPA MAKER: IMPA CATALOG</t>
+          <t>617182 SANDBAGS50KG</t>
         </is>
       </c>
       <c r="G124" s="49" t="n"/>
       <c r="H124" s="49" t="n"/>
       <c r="I124" s="48" t="n">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="J124" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>bags</t>
         </is>
       </c>
       <c r="K124" s="55" t="n"/>
@@ -4770,7 +4790,7 @@
       </c>
       <c r="B125" s="49" t="inlineStr">
         <is>
-          <t>GAUGE PRESSURE GLYCERINE BOTTM, DIRECT 0-25BAR 100MM G1/2IN</t>
+          <t>SHOVEL HOLDER, WALL-MOUNTED</t>
         </is>
       </c>
       <c r="C125" s="50" t="n"/>
@@ -4778,17 +4798,17 @@
       <c r="E125" s="49" t="n"/>
       <c r="F125" s="49" t="inlineStr">
         <is>
-          <t>653127 IMPA MAKER: IMPA CATALOG</t>
+          <t>617183 SHOVELHOLDERWALL</t>
         </is>
       </c>
       <c r="G125" s="49" t="n"/>
       <c r="H125" s="49" t="n"/>
       <c r="I125" s="48" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J125" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K125" s="55" t="n"/>
@@ -4802,7 +4822,7 @@
       </c>
       <c r="B126" s="49" t="inlineStr">
         <is>
-          <t>LADDER 2-EXTENSION ALUM-ALLOY, 4.5M</t>
+          <t>SNOW REMOVAL EQUIPMENT, HEAVY-DUTY SNOW PLOW</t>
         </is>
       </c>
       <c r="C126" s="50" t="n"/>
@@ -4810,7 +4830,7 @@
       <c r="E126" s="49" t="n"/>
       <c r="F126" s="49" t="inlineStr">
         <is>
-          <t>617110 IMPA MAKER: IMPA CATALOG</t>
+          <t>617184 SNOWPLOWHEAVYDUTY</t>
         </is>
       </c>
       <c r="G126" s="49" t="n"/>
@@ -4820,7 +4840,7 @@
       </c>
       <c r="J126" s="48" t="inlineStr">
         <is>
-          <t>SET</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K126" s="55" t="n"/>
@@ -4834,7 +4854,7 @@
       </c>
       <c r="B127" s="49" t="inlineStr">
         <is>
-          <t>LADDER PLATFORM ALUM-ALLOY, 1.2M</t>
+          <t>ROAD SIGNS, REFLECTIVE, CONSTRUCTION</t>
         </is>
       </c>
       <c r="C127" s="50" t="n"/>
@@ -4842,17 +4862,17 @@
       <c r="E127" s="49" t="n"/>
       <c r="F127" s="49" t="inlineStr">
         <is>
-          <t>617127 IMPA MAKER: IMPA CATALOG</t>
+          <t>617185 ROADSIGNSCONSTRUCTION</t>
         </is>
       </c>
       <c r="G127" s="49" t="n"/>
       <c r="H127" s="49" t="n"/>
       <c r="I127" s="48" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="J127" s="48" t="inlineStr">
         <is>
-          <t>SET</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K127" s="55" t="n"/>
@@ -4866,7 +4886,7 @@
       </c>
       <c r="B128" s="49" t="inlineStr">
         <is>
-          <t>GAUGE PRESSURE W/GLYCERINE, REAR/DIRECT 0-10BAR 63MM G1/4IN</t>
+          <t>TRAFFIC CONES, 750MM HEIGHT, ORANGE</t>
         </is>
       </c>
       <c r="C128" s="50" t="n"/>
@@ -4874,17 +4894,17 @@
       <c r="E128" s="49" t="n"/>
       <c r="F128" s="49" t="inlineStr">
         <is>
-          <t>653219 IMPA MAKER: IMPA CATALOG</t>
+          <t>617186 TRAFFICCONESORANGE</t>
         </is>
       </c>
       <c r="G128" s="49" t="n"/>
       <c r="H128" s="49" t="n"/>
       <c r="I128" s="48" t="n">
-        <v>2</v>
+        <v>50</v>
       </c>
       <c r="J128" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K128" s="55" t="n"/>
@@ -4898,7 +4918,7 @@
       </c>
       <c r="B129" s="49" t="inlineStr">
         <is>
-          <t>LETTER SET STEEL ALPHABET 27S, 5MM</t>
+          <t>CONSTRUCTION BARRIERS, 2M LENGTH</t>
         </is>
       </c>
       <c r="C129" s="50" t="n"/>
@@ -4906,17 +4926,17 @@
       <c r="E129" s="49" t="n"/>
       <c r="F129" s="49" t="inlineStr">
         <is>
-          <t>613106 IMPA MAKER: IMPA CATALOG</t>
+          <t>617187 CONSTRUCTIONBARRIERS</t>
         </is>
       </c>
       <c r="G129" s="49" t="n"/>
       <c r="H129" s="49" t="n"/>
       <c r="I129" s="48" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="J129" s="48" t="inlineStr">
         <is>
-          <t>SET</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K129" s="55" t="n"/>
@@ -4930,7 +4950,7 @@
       </c>
       <c r="B130" s="49" t="inlineStr">
         <is>
-          <t>FIGURE SET STEEL 9S 5MM</t>
+          <t>EARTHQUAKE-PROOF BRACING SYSTEMS, STEEL</t>
         </is>
       </c>
       <c r="C130" s="50" t="n"/>
@@ -4938,17 +4958,17 @@
       <c r="E130" s="49" t="n"/>
       <c r="F130" s="49" t="inlineStr">
         <is>
-          <t>613121 IMPA MAKER: IMPA CATALOG</t>
+          <t>617188 EARTHQUAKEBRACINGSTEEL</t>
         </is>
       </c>
       <c r="G130" s="49" t="n"/>
       <c r="H130" s="49" t="n"/>
       <c r="I130" s="48" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="J130" s="48" t="inlineStr">
         <is>
-          <t>SET</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K130" s="55" t="n"/>
@@ -4962,7 +4982,7 @@
       </c>
       <c r="B131" s="49" t="inlineStr">
         <is>
-          <t>VISE JAW PAD ALUM 100MM, WITH MAGNET</t>
+          <t>INDUSTRIAL SEALANT, SILICONE, 500ML</t>
         </is>
       </c>
       <c r="C131" s="50" t="n"/>
@@ -4970,17 +4990,17 @@
       <c r="E131" s="49" t="n"/>
       <c r="F131" s="49" t="inlineStr">
         <is>
-          <t>613791 IMPA MAKER: IMPA CATALOG</t>
+          <t>617189 SEALANTINDUSTRIAL</t>
         </is>
       </c>
       <c r="G131" s="49" t="n"/>
       <c r="H131" s="49" t="n"/>
       <c r="I131" s="48" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="J131" s="48" t="inlineStr">
         <is>
-          <t>PRS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K131" s="55" t="n"/>
@@ -4994,7 +5014,7 @@
       </c>
       <c r="B132" s="49" t="inlineStr">
         <is>
-          <t>SEWING MACHINE PORTABLE 220V</t>
+          <t>ROOF FLASHING, ALUMINUM, 0.5MM THICK</t>
         </is>
       </c>
       <c r="C132" s="50" t="n"/>
@@ -5002,17 +5022,17 @@
       <c r="E132" s="49" t="n"/>
       <c r="F132" s="49" t="inlineStr">
         <is>
-          <t>174732 IMPA MAKER: IMPA CATALOG</t>
+          <t>617190 ROOFFLASHING0.5MM</t>
         </is>
       </c>
       <c r="G132" s="49" t="n"/>
       <c r="H132" s="49" t="n"/>
       <c r="I132" s="48" t="n">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="J132" s="48" t="inlineStr">
         <is>
-          <t>SET</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K132" s="55" t="n"/>
@@ -5026,7 +5046,7 @@
       </c>
       <c r="B133" s="49" t="inlineStr">
         <is>
-          <t>SEWING NEEDLE NO.9 10S</t>
+          <t>GUTTER SYSTEM COMPONENTS, PVC, 100MM DIAMETER</t>
         </is>
       </c>
       <c r="C133" s="50" t="n"/>
@@ -5034,17 +5054,17 @@
       <c r="E133" s="49" t="n"/>
       <c r="F133" s="49" t="inlineStr">
         <is>
-          <t>174741 IMPA MAKER: IMPA CATALOG</t>
+          <t>617191 GUTTERCOMPONENTS100MM</t>
         </is>
       </c>
       <c r="G133" s="49" t="n"/>
       <c r="H133" s="49" t="n"/>
       <c r="I133" s="48" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="J133" s="48" t="inlineStr">
         <is>
-          <t>PKT</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K133" s="55" t="n"/>
@@ -5058,7 +5078,7 @@
       </c>
       <c r="B134" s="49" t="inlineStr">
         <is>
-          <t>SEWING NEEDLE NO.11 10S</t>
+          <t>DOWNSPOUTS, PVC, 80MM DIAMETER</t>
         </is>
       </c>
       <c r="C134" s="50" t="n"/>
@@ -5066,17 +5086,17 @@
       <c r="E134" s="49" t="n"/>
       <c r="F134" s="49" t="inlineStr">
         <is>
-          <t>174742 IMPA MAKER: IMPA CATALOG</t>
+          <t>617192 DOWNSPOUTSPVC80MM</t>
         </is>
       </c>
       <c r="G134" s="49" t="n"/>
       <c r="H134" s="49" t="n"/>
       <c r="I134" s="48" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="J134" s="48" t="inlineStr">
         <is>
-          <t>PKT</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K134" s="55" t="n"/>
@@ -5090,15 +5110,19 @@
       </c>
       <c r="B135" s="49" t="inlineStr">
         <is>
-          <t>SEWING NEEDLE NO.14 10S</t>
+          <t>PRESSURE WASHER, 3000 PSI</t>
         </is>
       </c>
       <c r="C135" s="50" t="n"/>
       <c r="D135" s="51" t="n"/>
-      <c r="E135" s="49" t="n"/>
+      <c r="E135" s="49" t="inlineStr">
+        <is>
+          <t>SH-FB-M/L</t>
+        </is>
+      </c>
       <c r="F135" s="49" t="inlineStr">
         <is>
-          <t>174743 IMPA MAKER: IMPA CATALOG</t>
+          <t>617193 PRESSUREWASHER3000PSI</t>
         </is>
       </c>
       <c r="G135" s="49" t="n"/>
@@ -5108,7 +5132,7 @@
       </c>
       <c r="J135" s="48" t="inlineStr">
         <is>
-          <t>PKT</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K135" s="55" t="n"/>
@@ -5122,7 +5146,7 @@
       </c>
       <c r="B136" s="49" t="inlineStr">
         <is>
-          <t>SEWING NEEDLE NO.16 10S</t>
+          <t>PRESSURE WASHER ACCESSORIES, 10M HOSE</t>
         </is>
       </c>
       <c r="C136" s="50" t="n"/>
@@ -5130,7 +5154,7 @@
       <c r="E136" s="49" t="n"/>
       <c r="F136" s="49" t="inlineStr">
         <is>
-          <t>174744 IMPA MAKER: IMPA CATALOG</t>
+          <t>617194 PRESSUREWASHERHOSE10M</t>
         </is>
       </c>
       <c r="G136" s="49" t="n"/>
@@ -5140,7 +5164,7 @@
       </c>
       <c r="J136" s="48" t="inlineStr">
         <is>
-          <t>PKT</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K136" s="55" t="n"/>
@@ -5154,7 +5178,7 @@
       </c>
       <c r="B137" s="49" t="inlineStr">
         <is>
-          <t>SEWING THREAD 200M</t>
+          <t>ASPHALT SEALANT, 25KG BUCKET</t>
         </is>
       </c>
       <c r="C137" s="50" t="n"/>
@@ -5162,17 +5186,17 @@
       <c r="E137" s="49" t="n"/>
       <c r="F137" s="49" t="inlineStr">
         <is>
-          <t>174752 IMPA MAKER: IMPA CATALOG</t>
+          <t>617195 ASPHALTSEALANT25KG</t>
         </is>
       </c>
       <c r="G137" s="49" t="n"/>
       <c r="H137" s="49" t="n"/>
       <c r="I137" s="48" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="J137" s="48" t="inlineStr">
         <is>
-          <t>RLS</t>
+          <t>buckets</t>
         </is>
       </c>
       <c r="K137" s="55" t="n"/>
@@ -5186,7 +5210,7 @@
       </c>
       <c r="B138" s="49" t="inlineStr">
         <is>
-          <t>GLUE GENERAL PURPOSE 100GRM</t>
+          <t>ASPHALT PAVING TOOLS, SQUARE EDGED RAKES</t>
         </is>
       </c>
       <c r="C138" s="50" t="n"/>
@@ -5194,7 +5218,7 @@
       <c r="E138" s="49" t="n"/>
       <c r="F138" s="49" t="inlineStr">
         <is>
-          <t>812701 IMPA MAKER: IMPA CATALOG</t>
+          <t>617196 ASPHALTPAVINGTOOLS</t>
         </is>
       </c>
       <c r="G138" s="49" t="n"/>
@@ -5204,7 +5228,7 @@
       </c>
       <c r="J138" s="48" t="inlineStr">
         <is>
-          <t>TUB</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K138" s="55" t="n"/>
@@ -5218,7 +5242,7 @@
       </c>
       <c r="B139" s="49" t="inlineStr">
         <is>
-          <t>GLUE GENERAL PURPOSE 1KG</t>
+          <t>COLD PATCH ASPHALT, 25KG BAG</t>
         </is>
       </c>
       <c r="C139" s="50" t="n"/>
@@ -5226,17 +5250,17 @@
       <c r="E139" s="49" t="n"/>
       <c r="F139" s="49" t="inlineStr">
         <is>
-          <t>812703 IMPA MAKER: IMPA CATALOG</t>
+          <t>617197 COLDPATCHASPHALT25KG</t>
         </is>
       </c>
       <c r="G139" s="49" t="n"/>
       <c r="H139" s="49" t="n"/>
       <c r="I139" s="48" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="J139" s="48" t="inlineStr">
         <is>
-          <t>CAN</t>
+          <t>bags</t>
         </is>
       </c>
       <c r="K139" s="55" t="n"/>
@@ -5250,7 +5274,7 @@
       </c>
       <c r="B140" s="49" t="inlineStr">
         <is>
-          <t>CYLINDER MORTISE LOCK, WITH LEVER HANDLE OHS#2320</t>
+          <t>ROAD MARKING PAINT, YELLOW, 20L</t>
         </is>
       </c>
       <c r="C140" s="50" t="n"/>
@@ -5258,17 +5282,17 @@
       <c r="E140" s="49" t="n"/>
       <c r="F140" s="49" t="inlineStr">
         <is>
-          <t>490113 IMPA MAKER: IMPA CATALOG</t>
+          <t>617198 ROADMARKINGPAINTYELLOW</t>
         </is>
       </c>
       <c r="G140" s="49" t="n"/>
       <c r="H140" s="49" t="n"/>
       <c r="I140" s="48" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="J140" s="48" t="inlineStr">
         <is>
-          <t>SET</t>
+          <t>cans</t>
         </is>
       </c>
       <c r="K140" s="55" t="n"/>
@@ -5282,7 +5306,7 @@
       </c>
       <c r="B141" s="49" t="inlineStr">
         <is>
-          <t>CLEANER DRAIN PIPE 1KG</t>
+          <t>ASPHALT RAKE, STEEL, 1M WIDTH</t>
         </is>
       </c>
       <c r="C141" s="50" t="n"/>
@@ -5290,17 +5314,17 @@
       <c r="E141" s="49" t="n"/>
       <c r="F141" s="49" t="inlineStr">
         <is>
-          <t>550342 IMPA MAKER: IMPA CATALOG</t>
+          <t>617199 ASPHALTRAKESTEEL1M</t>
         </is>
       </c>
       <c r="G141" s="49" t="n"/>
       <c r="H141" s="49" t="n"/>
       <c r="I141" s="48" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="J141" s="48" t="inlineStr">
         <is>
-          <t>BTL</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K141" s="55" t="n"/>
@@ -5314,7 +5338,7 @@
       </c>
       <c r="B142" s="49" t="inlineStr">
         <is>
-          <t>CLEANER &amp; POLISH SPRAY, ST/STEEL 420ML</t>
+          <t>EARTH AUGER, 52CC, 2-STROKE</t>
         </is>
       </c>
       <c r="C142" s="50" t="n"/>
@@ -5322,17 +5346,17 @@
       <c r="E142" s="49" t="n"/>
       <c r="F142" s="49" t="inlineStr">
         <is>
-          <t>550355 IMPA MAKER: IMPA CATALOG</t>
+          <t>617200 EARTHAUGER52CC</t>
         </is>
       </c>
       <c r="G142" s="49" t="n"/>
       <c r="H142" s="49" t="n"/>
       <c r="I142" s="48" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="J142" s="48" t="inlineStr">
         <is>
-          <t>TIN</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K142" s="55" t="n"/>
@@ -5346,7 +5370,7 @@
       </c>
       <c r="B143" s="49" t="inlineStr">
         <is>
-          <t>SODA CAUSTIC FLAKE 500GRM</t>
+          <t>POST HOLE DIGGER, MANUAL</t>
         </is>
       </c>
       <c r="C143" s="50" t="n"/>
@@ -5354,17 +5378,17 @@
       <c r="E143" s="49" t="n"/>
       <c r="F143" s="49" t="inlineStr">
         <is>
-          <t>550871 IMPA MAKER: IMPA CATALOG</t>
+          <t>617201 POSTHOLEDIGGERMANUAL</t>
         </is>
       </c>
       <c r="G143" s="49" t="n"/>
       <c r="H143" s="49" t="n"/>
       <c r="I143" s="48" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="J143" s="48" t="inlineStr">
         <is>
-          <t>CAN</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K143" s="55" t="n"/>
@@ -5378,7 +5402,7 @@
       </c>
       <c r="B144" s="49" t="inlineStr">
         <is>
-          <t>PART FOR TUMBLER MORTISE LOCK,OHS#2410 #(2)-16 LV HUB SPRING</t>
+          <t>HAND TAMPING TOOL, STEEL, 2KG</t>
         </is>
       </c>
       <c r="C144" s="50" t="n"/>
@@ -5386,7 +5410,7 @@
       <c r="E144" s="49" t="n"/>
       <c r="F144" s="49" t="inlineStr">
         <is>
-          <t>490361 IMPA MAKER: IMPA CATALOG</t>
+          <t>617202 HANDTAMPINGTOOLSTEEL</t>
         </is>
       </c>
       <c r="G144" s="49" t="n"/>
@@ -5396,7 +5420,7 @@
       </c>
       <c r="J144" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K144" s="55" t="n"/>
@@ -5410,7 +5434,7 @@
       </c>
       <c r="B145" s="49" t="inlineStr">
         <is>
-          <t>PART FOR TUMBLER MORTISE LOCK,OHS#2410 #2-17 LATCH BOLT SPR.</t>
+          <t>SOIL TESTING KIT, DIGITAL METER</t>
         </is>
       </c>
       <c r="C145" s="50" t="n"/>
@@ -5418,17 +5442,17 @@
       <c r="E145" s="49" t="n"/>
       <c r="F145" s="49" t="inlineStr">
         <is>
-          <t>490362 IMPA MAKER: IMPA CATALOG</t>
+          <t>617203 SOILTESTKITDIGITAL</t>
         </is>
       </c>
       <c r="G145" s="49" t="n"/>
       <c r="H145" s="49" t="n"/>
       <c r="I145" s="48" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J145" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K145" s="55" t="n"/>
@@ -5442,7 +5466,7 @@
       </c>
       <c r="B146" s="49" t="inlineStr">
         <is>
-          <t>PART FOR TUMBLER MORTISE LOCK,OHS#2410 #(2)-18 THUM.HUB SPR.</t>
+          <t>DRAINAGE PIPE, PVC, 100MM DIAMETER</t>
         </is>
       </c>
       <c r="C146" s="50" t="n"/>
@@ -5450,17 +5474,17 @@
       <c r="E146" s="49" t="n"/>
       <c r="F146" s="49" t="inlineStr">
         <is>
-          <t>490363 IMPA MAKER: IMPA CATALOG</t>
+          <t>617204 DRAINAGEPIPEPVC100MM</t>
         </is>
       </c>
       <c r="G146" s="49" t="n"/>
       <c r="H146" s="49" t="n"/>
       <c r="I146" s="48" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="J146" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K146" s="55" t="n"/>
@@ -5474,7 +5498,7 @@
       </c>
       <c r="B147" s="49" t="inlineStr">
         <is>
-          <t>PART FOR TUMBLER MORTISE LOCK,OHS#2410 #(2)-19 THUMBLER SPR.</t>
+          <t>EROSION CONTROL FABRIC, 1M X 50M</t>
         </is>
       </c>
       <c r="C147" s="50" t="n"/>
@@ -5482,7 +5506,7 @@
       <c r="E147" s="49" t="n"/>
       <c r="F147" s="49" t="inlineStr">
         <is>
-          <t>490364 IMPA MAKER: IMPA CATALOG</t>
+          <t>617205 EROSIONFABRIC1MX50M</t>
         </is>
       </c>
       <c r="G147" s="49" t="n"/>
@@ -5492,7 +5516,7 @@
       </c>
       <c r="J147" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>rolls</t>
         </is>
       </c>
       <c r="K147" s="55" t="n"/>
@@ -5506,7 +5530,7 @@
       </c>
       <c r="B148" s="49" t="inlineStr">
         <is>
-          <t>STEP REPAIR HARD WOOD FOR, JIS PILOT LADDER 525X115X25MM</t>
+          <t>GEOTEXTILE FABRIC, 100GSM, 3M X 3M</t>
         </is>
       </c>
       <c r="C148" s="50" t="n"/>
@@ -5514,17 +5538,17 @@
       <c r="E148" s="49" t="n"/>
       <c r="F148" s="49" t="inlineStr">
         <is>
-          <t>232014 IMPA MAKER: IMPA CATALOG</t>
+          <t>617206 GEOTEXTILEFABRIC100GSM</t>
         </is>
       </c>
       <c r="G148" s="49" t="n"/>
       <c r="H148" s="49" t="n"/>
       <c r="I148" s="48" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="J148" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K148" s="55" t="n"/>
@@ -5538,7 +5562,7 @@
       </c>
       <c r="B149" s="49" t="inlineStr">
         <is>
-          <t>STEP PREVENTER REPAIR WOOD F/JIS PILOT LADDER 1800X115X25MM</t>
+          <t>CONSTRUCTION SAFETY NETS, 10M X 10M</t>
         </is>
       </c>
       <c r="C149" s="50" t="n"/>
@@ -5546,17 +5570,17 @@
       <c r="E149" s="49" t="n"/>
       <c r="F149" s="49" t="inlineStr">
         <is>
-          <t>232015 IMPA MAKER: IMPA CATALOG</t>
+          <t>617207 SAFETYNETS10MX10M</t>
         </is>
       </c>
       <c r="G149" s="49" t="n"/>
       <c r="H149" s="49" t="n"/>
       <c r="I149" s="48" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J149" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K149" s="55" t="n"/>
@@ -5570,7 +5594,7 @@
       </c>
       <c r="B150" s="49" t="inlineStr">
         <is>
-          <t>TURNBUCKLE FRAME GALV, EYE&amp;HOOK 9MMX150MM</t>
+          <t>FIRE EXTINGUISHER, ABC, 4KG</t>
         </is>
       </c>
       <c r="C150" s="50" t="n"/>
@@ -5578,17 +5602,17 @@
       <c r="E150" s="49" t="n"/>
       <c r="F150" s="49" t="inlineStr">
         <is>
-          <t>230548 IMPA MAKER: IMPA CATALOG</t>
+          <t>617208 FIREEXTINGUISHERABC4KG</t>
         </is>
       </c>
       <c r="G150" s="49" t="n"/>
       <c r="H150" s="49" t="n"/>
       <c r="I150" s="48" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="J150" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K150" s="55" t="n"/>
@@ -5602,7 +5626,7 @@
       </c>
       <c r="B151" s="49" t="inlineStr">
         <is>
-          <t>GREASE GUN W/RIDGID PIPE, FOR AIR GREASE PUMP</t>
+          <t>EMERGENCY FIRST AID KIT, 100-PIECE</t>
         </is>
       </c>
       <c r="C151" s="50" t="n"/>
@@ -5610,17 +5634,17 @@
       <c r="E151" s="49" t="n"/>
       <c r="F151" s="49" t="inlineStr">
         <is>
-          <t>617414 IMPA MAKER: IMPA CATALOG</t>
+          <t>617209 FIRSTAIDKIT100PC</t>
         </is>
       </c>
       <c r="G151" s="49" t="n"/>
       <c r="H151" s="49" t="n"/>
       <c r="I151" s="48" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J151" s="48" t="inlineStr">
         <is>
-          <t>SET</t>
+          <t>kits</t>
         </is>
       </c>
       <c r="K151" s="55" t="n"/>
@@ -5634,7 +5658,7 @@
       </c>
       <c r="B152" s="49" t="inlineStr">
         <is>
-          <t>GREASE FITTING 4-JAW, FOR AIR GREASE PUMP</t>
+          <t>FLASHLIGHT, RECHARGEABLE, 1000LM</t>
         </is>
       </c>
       <c r="C152" s="50" t="n"/>
@@ -5642,17 +5666,17 @@
       <c r="E152" s="49" t="n"/>
       <c r="F152" s="49" t="inlineStr">
         <is>
-          <t>617419 IMPA MAKER: IMPA CATALOG</t>
+          <t>617210 FLASHLIGHT1000LM</t>
         </is>
       </c>
       <c r="G152" s="49" t="n"/>
       <c r="H152" s="49" t="n"/>
       <c r="I152" s="48" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="J152" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K152" s="55" t="n"/>
@@ -5666,7 +5690,7 @@
       </c>
       <c r="B153" s="49" t="inlineStr">
         <is>
-          <t>STEP DRILL #ST-2 6-18MM</t>
+          <t>WORKBENCH, METAL, 1200X600MM</t>
         </is>
       </c>
       <c r="C153" s="50" t="n"/>
@@ -5674,17 +5698,17 @@
       <c r="E153" s="49" t="n"/>
       <c r="F153" s="49" t="inlineStr">
         <is>
-          <t>633802 IMPA MAKER: IMPA CATALOG</t>
+          <t>617211 WORKBENCHMETAL1200X600</t>
         </is>
       </c>
       <c r="G153" s="49" t="n"/>
       <c r="H153" s="49" t="n"/>
       <c r="I153" s="48" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J153" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K153" s="55" t="n"/>
@@ -5698,7 +5722,7 @@
       </c>
       <c r="B154" s="49" t="inlineStr">
         <is>
-          <t>GREASE NIPPLE STRAIGHT A-TYPE, PT 3/8 PLATED STEEL</t>
+          <t>HYDRAULIC CONCRETE BREAKER, 15KG</t>
         </is>
       </c>
       <c r="C154" s="50" t="n"/>
@@ -5706,17 +5730,17 @@
       <c r="E154" s="49" t="n"/>
       <c r="F154" s="49" t="inlineStr">
         <is>
-          <t>617609 IMPA MAKER: IMPA CATALOG</t>
+          <t>617212 CONCRETEBREAKER15KG</t>
         </is>
       </c>
       <c r="G154" s="49" t="n"/>
       <c r="H154" s="49" t="n"/>
       <c r="I154" s="48" t="n">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="J154" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K154" s="55" t="n"/>
@@ -5730,25 +5754,29 @@
       </c>
       <c r="B155" s="49" t="inlineStr">
         <is>
-          <t>FLOATING DISC</t>
+          <t>CONCRETE FORMWORK SYSTEM, METAL, 3M HEIGHT</t>
         </is>
       </c>
       <c r="C155" s="50" t="n"/>
       <c r="D155" s="51" t="n"/>
-      <c r="E155" s="49" t="n"/>
+      <c r="E155" s="49" t="inlineStr">
+        <is>
+          <t>FPE-RE-2M</t>
+        </is>
+      </c>
       <c r="F155" s="49" t="inlineStr">
         <is>
-          <t>FOR 250A AIR HEAD,ST/STEEL MAKER: HYUNDAI HEAVY INDUSTRIES CO., LTD. (HHI)</t>
+          <t>617213 CONCRETEFORMSYSTEM3M</t>
         </is>
       </c>
       <c r="G155" s="49" t="n"/>
       <c r="H155" s="49" t="n"/>
       <c r="I155" s="48" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="J155" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K155" s="55" t="n"/>
@@ -5762,7 +5790,7 @@
       </c>
       <c r="B156" s="49" t="inlineStr">
         <is>
-          <t>FLOATING DISC</t>
+          <t>LASER DISTANCE MEASURER, 50M RANGE</t>
         </is>
       </c>
       <c r="C156" s="50" t="n"/>
@@ -5770,17 +5798,17 @@
       <c r="E156" s="49" t="n"/>
       <c r="F156" s="49" t="inlineStr">
         <is>
-          <t>FOR 300A AIR HEAD,ST/STEEL MAKER: ROLLS-ROYCE., LTD. (HHI)</t>
+          <t>617214 LASERDISTANCE50M</t>
         </is>
       </c>
       <c r="G156" s="49" t="n"/>
       <c r="H156" s="49" t="n"/>
       <c r="I156" s="48" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J156" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K156" s="55" t="n"/>
@@ -5794,7 +5822,7 @@
       </c>
       <c r="B157" s="49" t="inlineStr">
         <is>
-          <t>WRENCH SET OPEN &amp; 12-POINT BOX, 6X6 TO 32X32MM 16S</t>
+          <t>NOISE BARRIERS, 2M HEIGHT</t>
         </is>
       </c>
       <c r="C157" s="50" t="n"/>
@@ -5802,17 +5830,17 @@
       <c r="E157" s="49" t="n"/>
       <c r="F157" s="49" t="inlineStr">
         <is>
-          <t>610536 IMPA MAKER: IMPA CATALOG</t>
+          <t>617215 NOISEBARRIERS2M</t>
         </is>
       </c>
       <c r="G157" s="49" t="n"/>
       <c r="H157" s="49" t="n"/>
       <c r="I157" s="48" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J157" s="48" t="inlineStr">
         <is>
-          <t>SET</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K157" s="55" t="n"/>
@@ -5826,27 +5854,25 @@
       </c>
       <c r="B158" s="49" t="inlineStr">
         <is>
-          <t>WRENCH STRIKING RING 12P 24MM, ST/STEEL</t>
+          <t>INSULATED WIRE, 2.5MM², 100M ROLL</t>
         </is>
       </c>
       <c r="C158" s="50" t="n"/>
       <c r="D158" s="51" t="n"/>
-      <c r="E158" s="49" t="n">
-        <v>61234</v>
-      </c>
+      <c r="E158" s="49" t="n"/>
       <c r="F158" s="49" t="inlineStr">
         <is>
-          <t>616085 IMPA MAKER: IMPA CATALOG</t>
+          <t>617216 INSULATEDWIRE2.5MM100M</t>
         </is>
       </c>
       <c r="G158" s="49" t="n"/>
       <c r="H158" s="49" t="n"/>
       <c r="I158" s="48" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="J158" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>rolls</t>
         </is>
       </c>
       <c r="K158" s="55" t="n"/>
@@ -5860,27 +5886,25 @@
       </c>
       <c r="B159" s="49" t="inlineStr">
         <is>
-          <t>WRENCH STRIKING RING 12P 27MM, ST/STEEL</t>
+          <t>ELECTRICAL CONDUIT, PVC, 20MM DIAMETER</t>
         </is>
       </c>
       <c r="C159" s="50" t="n"/>
       <c r="D159" s="51" t="n"/>
-      <c r="E159" s="49" t="n">
-        <v>61235</v>
-      </c>
+      <c r="E159" s="49" t="n"/>
       <c r="F159" s="49" t="inlineStr">
         <is>
-          <t>616086 IMPA MAKER: IMPA CATALOG</t>
+          <t>617217 ELECTRICALCONDUITPVC20MM</t>
         </is>
       </c>
       <c r="G159" s="49" t="n"/>
       <c r="H159" s="49" t="n"/>
       <c r="I159" s="48" t="n">
-        <v>2</v>
+        <v>50</v>
       </c>
       <c r="J159" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K159" s="55" t="n"/>
@@ -5894,25 +5918,29 @@
       </c>
       <c r="B160" s="49" t="inlineStr">
         <is>
-          <t>GASKET FOR FLEXIBLE PIPE, COUPLING WITH FURTHER DETAIL</t>
+          <t>ELECTRICAL JUNCTION BOX, 200X200MM</t>
         </is>
       </c>
       <c r="C160" s="50" t="n"/>
       <c r="D160" s="51" t="n"/>
-      <c r="E160" s="49" t="n"/>
+      <c r="E160" s="49" t="inlineStr">
+        <is>
+          <t>FT-200X200</t>
+        </is>
+      </c>
       <c r="F160" s="49" t="inlineStr">
         <is>
-          <t>735036 IMPA MAKER: IMPA CATALOG</t>
+          <t>617218 JUNCTIONBOX200X200MM</t>
         </is>
       </c>
       <c r="G160" s="49" t="n"/>
       <c r="H160" s="49" t="n"/>
       <c r="I160" s="48" t="n">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="J160" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K160" s="55" t="n"/>
@@ -5926,7 +5954,7 @@
       </c>
       <c r="B161" s="49" t="inlineStr">
         <is>
-          <t>TAPE OIL GAUGE ST/STEEL, METRIC 30M</t>
+          <t>CIRCUIT BREAKERS, 16A, SINGLE POLE</t>
         </is>
       </c>
       <c r="C161" s="50" t="n"/>
@@ -5934,17 +5962,17 @@
       <c r="E161" s="49" t="n"/>
       <c r="F161" s="49" t="inlineStr">
         <is>
-          <t>650873 IMPA MAKER: IMPA CATALOG</t>
+          <t>617219 CIRCUITBREAKERS16A</t>
         </is>
       </c>
       <c r="G161" s="49" t="n"/>
       <c r="H161" s="49" t="n"/>
       <c r="I161" s="48" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="J161" s="48" t="inlineStr">
         <is>
-          <t>PCS</t>
+          <t>pcs</t>
         </is>
       </c>
       <c r="K161" s="55" t="n"/>
@@ -6036,19 +6064,50 @@
       <c r="M166" s="58" t="n"/>
       <c r="N166" s="58" t="n"/>
     </row>
-    <row r="167" ht="245" customHeight="1">
+    <row r="167" ht="667" customHeight="1">
       <c r="A167" s="45" t="n"/>
       <c r="B167" s="31" t="inlineStr">
         <is>
-          <t>ITEM 2 - CURTAIN SHOWER - 2 METERS LONG. 
-ITEM 120 - SCREW TAPPING WITH FURTHER, DETAILS: 
-TAPPING SCREW - STAINLESS STEEL - CROSS RECESSED BINDING HEAD - SIZE=3.5MM - LENGHT = 25MM - 100 PCS 
-TAPPING SCREW - STAINLESS STEEL - CROSS RECESSED BINDING HEAD - SIZE=3.5MM - LENGHT = 32MM - 100 PCS 
-TAPPING SCREW - STAINLESS STEEL - CROSS RECESSED BINDING HEAD - SIZE=3.5MM - LENGHT = 50MM - 100 PCS 
-ITEM 131 - SEWING MACHINE PORTABLE 220V - CAPABILITY TO SEWING CANVAS, COTTON, JEANS AND OTHET MATERIALS UP TO 4MM THICKNESS. 
-ITEM 139 - CYLINDER MORTISE LOCK, WITH LEVER HANDLE OHS#2320 - 1 right hand and 1 left hand of lock. 
-ITEM 151 - PLEASE PROVIDE STAINLESS STEEL TURNBUCKLES. 
-ITEM 161 - PLEASE PROVIDE GASKETS FOR FLEXIBLE PIPE COUPLING AS FOLLOWS: 2(TWO)PCS - 100A, 6(SIX)PCS - 200A, 4(FOUR)PCS - 500A.</t>
+          <t>ITEM 2 - CONCRETE MIXER - 220V, 150L CAPACITY
+Details:
+Electric Concrete Mixer with 220V power supply
+150L drum capacity for mixing cement, sand, gravel, and water
+Suitable for medium-sized construction projects
+Durable steel frame and high-efficiency motor
+ITEM 15 - WELDING MACHINE, MIG/TIG - 250A
+Details:
+MIG and TIG welding capabilities for versatile use
+250A welding output for welding steel, aluminum, and other metals
+Adjustable amperage control for precise welding
+Includes foot pedal for TIG welding
+230V input voltage, suitable for most industrial environments
+ITEM 32 - SAFETY GLOVES, NITRILE - MEDIUM
+Details:
+Nitrile-coated gloves for maximum protection and comfort
+Provides resistance to oils, solvents, and chemicals
+Medium size for optimal fit
+Ideal for construction, automotive, and industrial work
+Pack of 10 pairs
+ITEM 42 - STEEL REBAR, 12MM DIAMETER, 6M LENGTH
+Details:
+High-strength steel rebar with 12mm diameter
+Standard 6-meter length for easy handling and installation
+Used for reinforcing concrete in construction projects
+Meets industry standards for strength and durability
+ITEM 56 - SCAFFOLDING COMPONENTS, ALUMINUM, 3M HEIGHT
+Details:
+Lightweight aluminum scaffolding for easy transport and setup
+3-meter height for standard building projects
+Ideal for interior and exterior work
+Includes locking pins and safety features for secure assembly
+Maximum load capacity of 150kg per section
+ITEM 70 - PAINT ROLLERS, 9”
+Details:
+9-inch rollers for large surface coverage
+Suitable for applying paint, primers, and stains
+High-density fabric for smooth, even application
+Comfortable handle design with anti-slip grip
+Pack of 5 rollers</t>
         </is>
       </c>
       <c r="C167" s="43" t="n"/>

</xml_diff>